<commit_message>
Added another victory blueprint and replaced the circus tent
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="16440" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Junk" sheetId="1" r:id="rId1"/>
@@ -82,9 +82,6 @@
     <t>Rockin' Skateboard</t>
   </si>
   <si>
-    <t>Colorful Circus Tent</t>
-  </si>
-  <si>
     <t>Nice Sweater</t>
   </si>
   <si>
@@ -410,9 +407,6 @@
   </si>
   <si>
     <t>"What's this sparkly thing? Maybe I can trade it in."</t>
-  </si>
-  <si>
-    <t>"A good find AND a wise business decision!"</t>
   </si>
   <si>
     <t>"Nothing says 'scram!' like a man with a flail."</t>
@@ -693,6 +687,12 @@
   </si>
   <si>
     <t>Bundle of Two-by-Fours</t>
+  </si>
+  <si>
+    <t>Naturally Lit Yurt</t>
+  </si>
+  <si>
+    <t>"You can never have too many windows in a yurt!"</t>
   </si>
 </sst>
 </file>
@@ -3046,10 +3046,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:GF58"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -3084,7 +3084,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="110" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E1" s="111" t="s">
         <v>3</v>
@@ -3099,34 +3099,34 @@
         <v>6</v>
       </c>
       <c r="I1" s="113" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J1" s="111" t="s">
+        <v>164</v>
+      </c>
+      <c r="K1" s="114" t="s">
+        <v>165</v>
+      </c>
+      <c r="L1" s="114" t="s">
         <v>166</v>
       </c>
-      <c r="K1" s="114" t="s">
+      <c r="M1" s="114" t="s">
         <v>167</v>
       </c>
-      <c r="L1" s="114" t="s">
+      <c r="N1" s="112" t="s">
+        <v>126</v>
+      </c>
+      <c r="O1" s="112" t="s">
         <v>168</v>
       </c>
-      <c r="M1" s="114" t="s">
+      <c r="P1" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="N1" s="112" t="s">
-        <v>127</v>
-      </c>
-      <c r="O1" s="112" t="s">
+      <c r="Q1" s="112" t="s">
         <v>170</v>
       </c>
-      <c r="P1" s="112" t="s">
+      <c r="R1" s="112" t="s">
         <v>171</v>
-      </c>
-      <c r="Q1" s="112" t="s">
-        <v>172</v>
-      </c>
-      <c r="R1" s="112" t="s">
-        <v>173</v>
       </c>
       <c r="S1" s="115"/>
       <c r="T1" s="115"/>
@@ -3310,7 +3310,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="120" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E2" s="121"/>
       <c r="F2" s="122"/>
@@ -3344,7 +3344,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="127" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E3" s="67"/>
       <c r="F3" s="72">
@@ -3380,7 +3380,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="127" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E4" s="67"/>
       <c r="F4" s="72">
@@ -3418,7 +3418,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="127" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E5" s="70">
         <v>3</v>
@@ -3454,7 +3454,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="127" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E6" s="67"/>
       <c r="F6" s="68"/>
@@ -3492,7 +3492,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="127" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E7" s="67"/>
       <c r="F7" s="72">
@@ -3532,7 +3532,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="127" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E8" s="70">
         <v>2</v>
@@ -3570,14 +3570,12 @@
         <v>10</v>
       </c>
       <c r="D9" s="127" t="s">
-        <v>131</v>
+        <v>203</v>
       </c>
       <c r="E9" s="70">
-        <v>2</v>
-      </c>
-      <c r="F9" s="72">
-        <v>2</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F9" s="68"/>
       <c r="G9" s="68"/>
       <c r="H9" s="68"/>
       <c r="I9" s="69"/>
@@ -3585,7 +3583,7 @@
         <v>1</v>
       </c>
       <c r="K9" s="71" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="L9" s="68"/>
       <c r="M9" s="68"/>
@@ -3606,13 +3604,15 @@
         <v>10</v>
       </c>
       <c r="D10" s="127" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E10" s="70">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F10" s="68"/>
-      <c r="G10" s="68"/>
+      <c r="G10" s="72">
+        <v>2</v>
+      </c>
       <c r="H10" s="68"/>
       <c r="I10" s="69"/>
       <c r="J10" s="70">
@@ -3640,30 +3640,34 @@
         <v>10</v>
       </c>
       <c r="D11" s="127" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E11" s="70">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" s="68"/>
-      <c r="G11" s="72">
-        <v>2</v>
-      </c>
-      <c r="H11" s="68"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="72">
+        <v>1</v>
+      </c>
       <c r="I11" s="69"/>
       <c r="J11" s="70">
         <v>1</v>
       </c>
       <c r="K11" s="71" t="s">
-        <v>17</v>
-      </c>
-      <c r="L11" s="68"/>
-      <c r="M11" s="68"/>
-      <c r="N11" s="73"/>
+        <v>14</v>
+      </c>
+      <c r="L11" s="72">
+        <v>1</v>
+      </c>
+      <c r="M11" s="71" t="s">
+        <v>18</v>
+      </c>
+      <c r="N11" s="72"/>
       <c r="O11" s="72"/>
-      <c r="P11" s="73"/>
+      <c r="P11" s="72"/>
       <c r="Q11" s="72"/>
-      <c r="R11" s="73"/>
+      <c r="R11" s="72"/>
     </row>
     <row r="12" spans="1:188" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="64" t="s">
@@ -3676,34 +3680,26 @@
         <v>10</v>
       </c>
       <c r="D12" s="127" t="s">
-        <v>204</v>
-      </c>
-      <c r="E12" s="70">
+        <v>131</v>
+      </c>
+      <c r="E12" s="67"/>
+      <c r="F12" s="72">
         <v>2</v>
       </c>
-      <c r="F12" s="68"/>
       <c r="G12" s="68"/>
       <c r="H12" s="72">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12" s="69"/>
-      <c r="J12" s="70">
-        <v>1</v>
-      </c>
-      <c r="K12" s="71" t="s">
-        <v>14</v>
-      </c>
-      <c r="L12" s="72">
-        <v>1</v>
-      </c>
-      <c r="M12" s="71" t="s">
-        <v>18</v>
-      </c>
-      <c r="N12" s="72"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="68"/>
+      <c r="L12" s="68"/>
+      <c r="M12" s="68"/>
+      <c r="N12" s="73"/>
       <c r="O12" s="72"/>
-      <c r="P12" s="72"/>
+      <c r="P12" s="73"/>
       <c r="Q12" s="72"/>
-      <c r="R12" s="72"/>
+      <c r="R12" s="73"/>
     </row>
     <row r="13" spans="1:188" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="64" t="s">
@@ -3718,24 +3714,32 @@
       <c r="D13" s="127" t="s">
         <v>133</v>
       </c>
-      <c r="E13" s="67"/>
-      <c r="F13" s="72">
+      <c r="E13" s="70">
         <v>2</v>
       </c>
+      <c r="F13" s="68"/>
       <c r="G13" s="68"/>
       <c r="H13" s="72">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I13" s="69"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="68"/>
-      <c r="L13" s="68"/>
-      <c r="M13" s="68"/>
-      <c r="N13" s="73"/>
+      <c r="J13" s="70">
+        <v>1</v>
+      </c>
+      <c r="K13" s="71" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" s="72">
+        <v>1</v>
+      </c>
+      <c r="M13" s="71" t="s">
+        <v>18</v>
+      </c>
+      <c r="N13" s="72"/>
       <c r="O13" s="72"/>
-      <c r="P13" s="73"/>
+      <c r="P13" s="72"/>
       <c r="Q13" s="72"/>
-      <c r="R13" s="73"/>
+      <c r="R13" s="72"/>
     </row>
     <row r="14" spans="1:188" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="64" t="s">
@@ -3748,13 +3752,15 @@
         <v>10</v>
       </c>
       <c r="D14" s="127" t="s">
-        <v>135</v>
-      </c>
-      <c r="E14" s="70">
+        <v>204</v>
+      </c>
+      <c r="E14" s="67"/>
+      <c r="F14" s="72">
         <v>2</v>
       </c>
-      <c r="F14" s="68"/>
-      <c r="G14" s="68"/>
+      <c r="G14" s="72">
+        <v>1</v>
+      </c>
       <c r="H14" s="72">
         <v>1</v>
       </c>
@@ -3763,19 +3769,15 @@
         <v>1</v>
       </c>
       <c r="K14" s="71" t="s">
-        <v>17</v>
-      </c>
-      <c r="L14" s="72">
-        <v>1</v>
-      </c>
-      <c r="M14" s="71" t="s">
-        <v>18</v>
-      </c>
-      <c r="N14" s="72"/>
+        <v>14</v>
+      </c>
+      <c r="L14" s="68"/>
+      <c r="M14" s="68"/>
+      <c r="N14" s="73"/>
       <c r="O14" s="72"/>
-      <c r="P14" s="72"/>
+      <c r="P14" s="73"/>
       <c r="Q14" s="72"/>
-      <c r="R14" s="72"/>
+      <c r="R14" s="73"/>
     </row>
     <row r="15" spans="1:188" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="64" t="s">
@@ -3788,14 +3790,14 @@
         <v>10</v>
       </c>
       <c r="D15" s="127" t="s">
-        <v>206</v>
+        <v>132</v>
       </c>
       <c r="E15" s="67"/>
       <c r="F15" s="72">
+        <v>1</v>
+      </c>
+      <c r="G15" s="72">
         <v>2</v>
-      </c>
-      <c r="G15" s="72">
-        <v>1</v>
       </c>
       <c r="H15" s="72">
         <v>1</v>
@@ -3805,7 +3807,7 @@
         <v>1</v>
       </c>
       <c r="K15" s="71" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L15" s="68"/>
       <c r="M15" s="68"/>
@@ -3829,21 +3831,17 @@
         <v>134</v>
       </c>
       <c r="E16" s="67"/>
-      <c r="F16" s="72">
-        <v>1</v>
-      </c>
-      <c r="G16" s="72">
-        <v>2</v>
-      </c>
+      <c r="F16" s="68"/>
+      <c r="G16" s="68"/>
       <c r="H16" s="72">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I16" s="69"/>
       <c r="J16" s="70">
         <v>1</v>
       </c>
       <c r="K16" s="71" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="L16" s="68"/>
       <c r="M16" s="68"/>
@@ -3864,21 +3862,19 @@
         <v>10</v>
       </c>
       <c r="D17" s="127" t="s">
-        <v>136</v>
-      </c>
-      <c r="E17" s="67"/>
-      <c r="F17" s="68"/>
+        <v>135</v>
+      </c>
+      <c r="E17" s="70">
+        <v>3</v>
+      </c>
+      <c r="F17" s="72">
+        <v>3</v>
+      </c>
       <c r="G17" s="68"/>
-      <c r="H17" s="72">
-        <v>3</v>
-      </c>
+      <c r="H17" s="68"/>
       <c r="I17" s="69"/>
-      <c r="J17" s="70">
-        <v>1</v>
-      </c>
-      <c r="K17" s="71" t="s">
-        <v>11</v>
-      </c>
+      <c r="J17" s="67"/>
+      <c r="K17" s="68"/>
       <c r="L17" s="68"/>
       <c r="M17" s="68"/>
       <c r="N17" s="73"/>
@@ -3898,19 +3894,23 @@
         <v>10</v>
       </c>
       <c r="D18" s="127" t="s">
-        <v>137</v>
-      </c>
-      <c r="E18" s="70">
+        <v>205</v>
+      </c>
+      <c r="E18" s="67"/>
+      <c r="F18" s="68"/>
+      <c r="G18" s="72">
         <v>3</v>
       </c>
-      <c r="F18" s="72">
-        <v>3</v>
-      </c>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
+      <c r="H18" s="72">
+        <v>1</v>
+      </c>
       <c r="I18" s="69"/>
-      <c r="J18" s="67"/>
-      <c r="K18" s="68"/>
+      <c r="J18" s="70">
+        <v>1</v>
+      </c>
+      <c r="K18" s="71" t="s">
+        <v>11</v>
+      </c>
       <c r="L18" s="68"/>
       <c r="M18" s="68"/>
       <c r="N18" s="73"/>
@@ -3930,66 +3930,62 @@
         <v>10</v>
       </c>
       <c r="D19" s="127" t="s">
-        <v>207</v>
+        <v>136</v>
       </c>
       <c r="E19" s="67"/>
-      <c r="F19" s="68"/>
+      <c r="F19" s="72">
+        <v>2</v>
+      </c>
       <c r="G19" s="72">
-        <v>3</v>
-      </c>
-      <c r="H19" s="72">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H19" s="68"/>
       <c r="I19" s="69"/>
       <c r="J19" s="70">
         <v>1</v>
       </c>
       <c r="K19" s="71" t="s">
-        <v>11</v>
-      </c>
-      <c r="L19" s="68"/>
-      <c r="M19" s="68"/>
-      <c r="N19" s="73"/>
+        <v>125</v>
+      </c>
+      <c r="L19" s="72"/>
+      <c r="M19" s="71"/>
+      <c r="N19" s="72"/>
       <c r="O19" s="72"/>
-      <c r="P19" s="73"/>
+      <c r="P19" s="72"/>
       <c r="Q19" s="72"/>
-      <c r="R19" s="73"/>
+      <c r="R19" s="72"/>
     </row>
     <row r="20" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="65" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C20" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="127" t="s">
-        <v>138</v>
-      </c>
-      <c r="E20" s="67"/>
+        <v>137</v>
+      </c>
+      <c r="E20" s="70">
+        <v>4</v>
+      </c>
       <c r="F20" s="72">
-        <v>2</v>
-      </c>
-      <c r="G20" s="72">
-        <v>2</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="G20" s="68"/>
       <c r="H20" s="68"/>
       <c r="I20" s="69"/>
-      <c r="J20" s="70">
-        <v>1</v>
-      </c>
-      <c r="K20" s="71" t="s">
-        <v>126</v>
-      </c>
-      <c r="L20" s="72"/>
-      <c r="M20" s="71"/>
-      <c r="N20" s="72"/>
+      <c r="J20" s="67"/>
+      <c r="K20" s="68"/>
+      <c r="L20" s="68"/>
+      <c r="M20" s="68"/>
+      <c r="N20" s="73"/>
       <c r="O20" s="72"/>
-      <c r="P20" s="72"/>
+      <c r="P20" s="73"/>
       <c r="Q20" s="72"/>
-      <c r="R20" s="72"/>
+      <c r="R20" s="73"/>
     </row>
     <row r="21" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="64" t="s">
@@ -4002,19 +3998,25 @@
         <v>10</v>
       </c>
       <c r="D21" s="127" t="s">
-        <v>139</v>
+        <v>211</v>
       </c>
       <c r="E21" s="70">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F21" s="72">
-        <v>3</v>
-      </c>
-      <c r="G21" s="68"/>
+        <v>1</v>
+      </c>
+      <c r="G21" s="72">
+        <v>1</v>
+      </c>
       <c r="H21" s="68"/>
       <c r="I21" s="69"/>
-      <c r="J21" s="67"/>
-      <c r="K21" s="68"/>
+      <c r="J21" s="70">
+        <v>1</v>
+      </c>
+      <c r="K21" s="71" t="s">
+        <v>36</v>
+      </c>
       <c r="L21" s="68"/>
       <c r="M21" s="68"/>
       <c r="N21" s="73"/>
@@ -4028,31 +4030,27 @@
         <v>8</v>
       </c>
       <c r="B22" s="65" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C22" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="127" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E22" s="70">
+        <v>3</v>
+      </c>
+      <c r="F22" s="72">
         <v>2</v>
       </c>
-      <c r="F22" s="72">
-        <v>1</v>
-      </c>
       <c r="G22" s="72">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H22" s="68"/>
       <c r="I22" s="69"/>
-      <c r="J22" s="70">
-        <v>1</v>
-      </c>
-      <c r="K22" s="71" t="s">
-        <v>37</v>
-      </c>
+      <c r="J22" s="67"/>
+      <c r="K22" s="68"/>
       <c r="L22" s="68"/>
       <c r="M22" s="68"/>
       <c r="N22" s="73"/>
@@ -4072,21 +4070,25 @@
         <v>10</v>
       </c>
       <c r="D23" s="127" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="E23" s="70">
         <v>3</v>
       </c>
-      <c r="F23" s="72">
-        <v>2</v>
-      </c>
+      <c r="F23" s="68"/>
       <c r="G23" s="72">
-        <v>2</v>
-      </c>
-      <c r="H23" s="68"/>
+        <v>1</v>
+      </c>
+      <c r="H23" s="72">
+        <v>1</v>
+      </c>
       <c r="I23" s="69"/>
-      <c r="J23" s="67"/>
-      <c r="K23" s="68"/>
+      <c r="J23" s="70">
+        <v>1</v>
+      </c>
+      <c r="K23" s="71" t="s">
+        <v>17</v>
+      </c>
       <c r="L23" s="68"/>
       <c r="M23" s="68"/>
       <c r="N23" s="73"/>
@@ -4106,25 +4108,21 @@
         <v>10</v>
       </c>
       <c r="D24" s="127" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E24" s="70">
-        <v>3</v>
-      </c>
-      <c r="F24" s="68"/>
-      <c r="G24" s="72">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F24" s="72">
+        <v>2</v>
+      </c>
+      <c r="G24" s="68"/>
       <c r="H24" s="72">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I24" s="69"/>
-      <c r="J24" s="70">
-        <v>1</v>
-      </c>
-      <c r="K24" s="71" t="s">
-        <v>17</v>
-      </c>
+      <c r="J24" s="67"/>
+      <c r="K24" s="68"/>
       <c r="L24" s="68"/>
       <c r="M24" s="68"/>
       <c r="N24" s="73"/>
@@ -4144,21 +4142,23 @@
         <v>10</v>
       </c>
       <c r="D25" s="127" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="E25" s="70">
         <v>2</v>
       </c>
-      <c r="F25" s="72">
-        <v>2</v>
-      </c>
+      <c r="F25" s="68"/>
       <c r="G25" s="68"/>
       <c r="H25" s="72">
         <v>2</v>
       </c>
       <c r="I25" s="69"/>
-      <c r="J25" s="67"/>
-      <c r="K25" s="68"/>
+      <c r="J25" s="70">
+        <v>2</v>
+      </c>
+      <c r="K25" s="71" t="s">
+        <v>11</v>
+      </c>
       <c r="L25" s="68"/>
       <c r="M25" s="68"/>
       <c r="N25" s="73"/>
@@ -4175,26 +4175,22 @@
         <v>41</v>
       </c>
       <c r="C26" s="66" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="D26" s="127" t="s">
-        <v>216</v>
-      </c>
-      <c r="E26" s="70">
-        <v>2</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="E26" s="67"/>
       <c r="F26" s="68"/>
-      <c r="G26" s="68"/>
+      <c r="G26" s="72">
+        <v>1</v>
+      </c>
       <c r="H26" s="72">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I26" s="69"/>
-      <c r="J26" s="70">
-        <v>2</v>
-      </c>
-      <c r="K26" s="71" t="s">
-        <v>11</v>
-      </c>
+      <c r="J26" s="67"/>
+      <c r="K26" s="68"/>
       <c r="L26" s="68"/>
       <c r="M26" s="68"/>
       <c r="N26" s="73"/>
@@ -4208,25 +4204,27 @@
         <v>8</v>
       </c>
       <c r="B27" s="65" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="66" t="s">
-        <v>43</v>
-      </c>
       <c r="D27" s="127" t="s">
-        <v>141</v>
-      </c>
-      <c r="E27" s="67"/>
+        <v>140</v>
+      </c>
+      <c r="E27" s="70">
+        <v>5</v>
+      </c>
       <c r="F27" s="68"/>
-      <c r="G27" s="72">
-        <v>1</v>
-      </c>
-      <c r="H27" s="72">
-        <v>3</v>
-      </c>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
       <c r="I27" s="69"/>
-      <c r="J27" s="67"/>
-      <c r="K27" s="68"/>
+      <c r="J27" s="70">
+        <v>2</v>
+      </c>
+      <c r="K27" s="71" t="s">
+        <v>14</v>
+      </c>
       <c r="L27" s="68"/>
       <c r="M27" s="68"/>
       <c r="N27" s="73"/>
@@ -4239,27 +4237,29 @@
       <c r="A28" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="65" t="s">
-        <v>44</v>
+      <c r="B28" s="139" t="s">
+        <v>220</v>
       </c>
       <c r="C28" s="66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D28" s="127" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E28" s="70">
-        <v>5</v>
-      </c>
-      <c r="F28" s="68"/>
+        <v>2</v>
+      </c>
+      <c r="F28" s="72">
+        <v>2</v>
+      </c>
       <c r="G28" s="68"/>
       <c r="H28" s="68"/>
       <c r="I28" s="69"/>
       <c r="J28" s="70">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K28" s="71" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L28" s="68"/>
       <c r="M28" s="68"/>
@@ -4273,29 +4273,29 @@
       <c r="A29" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="139" t="s">
-        <v>222</v>
+      <c r="B29" s="65" t="s">
+        <v>44</v>
       </c>
       <c r="C29" s="66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D29" s="127" t="s">
-        <v>143</v>
-      </c>
-      <c r="E29" s="70">
-        <v>2</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="E29" s="67"/>
       <c r="F29" s="72">
         <v>2</v>
       </c>
-      <c r="G29" s="68"/>
+      <c r="G29" s="72">
+        <v>2</v>
+      </c>
       <c r="H29" s="68"/>
       <c r="I29" s="69"/>
       <c r="J29" s="70">
         <v>1</v>
       </c>
       <c r="K29" s="71" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="L29" s="68"/>
       <c r="M29" s="68"/>
@@ -4313,22 +4313,24 @@
         <v>45</v>
       </c>
       <c r="C30" s="66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D30" s="127" t="s">
-        <v>144</v>
-      </c>
-      <c r="E30" s="67"/>
-      <c r="F30" s="72">
-        <v>2</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="E30" s="70">
+        <v>1</v>
+      </c>
+      <c r="F30" s="68"/>
       <c r="G30" s="72">
-        <v>2</v>
-      </c>
-      <c r="H30" s="68"/>
+        <v>1</v>
+      </c>
+      <c r="H30" s="72">
+        <v>1</v>
+      </c>
       <c r="I30" s="69"/>
       <c r="J30" s="70">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K30" s="71" t="s">
         <v>14</v>
@@ -4349,27 +4351,25 @@
         <v>46</v>
       </c>
       <c r="C31" s="66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D31" s="127" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E31" s="70">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F31" s="68"/>
       <c r="G31" s="72">
-        <v>1</v>
-      </c>
-      <c r="H31" s="72">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H31" s="68"/>
       <c r="I31" s="69"/>
       <c r="J31" s="70">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K31" s="71" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="L31" s="68"/>
       <c r="M31" s="68"/>
@@ -4387,15 +4387,15 @@
         <v>47</v>
       </c>
       <c r="C32" s="66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D32" s="127" t="s">
-        <v>146</v>
-      </c>
-      <c r="E32" s="70">
-        <v>3</v>
-      </c>
-      <c r="F32" s="68"/>
+        <v>145</v>
+      </c>
+      <c r="E32" s="67"/>
+      <c r="F32" s="72">
+        <v>2</v>
+      </c>
       <c r="G32" s="72">
         <v>2</v>
       </c>
@@ -4423,26 +4423,24 @@
         <v>48</v>
       </c>
       <c r="C33" s="66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D33" s="127" t="s">
-        <v>147</v>
-      </c>
-      <c r="E33" s="67"/>
+        <v>208</v>
+      </c>
+      <c r="E33" s="70">
+        <v>3</v>
+      </c>
       <c r="F33" s="72">
         <v>2</v>
       </c>
-      <c r="G33" s="72">
-        <v>2</v>
-      </c>
-      <c r="H33" s="68"/>
+      <c r="G33" s="68"/>
+      <c r="H33" s="72">
+        <v>1</v>
+      </c>
       <c r="I33" s="69"/>
-      <c r="J33" s="70">
-        <v>1</v>
-      </c>
-      <c r="K33" s="71" t="s">
-        <v>11</v>
-      </c>
+      <c r="J33" s="67"/>
+      <c r="K33" s="68"/>
       <c r="L33" s="68"/>
       <c r="M33" s="68"/>
       <c r="N33" s="73"/>
@@ -4459,20 +4457,20 @@
         <v>49</v>
       </c>
       <c r="C34" s="66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D34" s="127" t="s">
-        <v>210</v>
+        <v>146</v>
       </c>
       <c r="E34" s="70">
-        <v>3</v>
-      </c>
-      <c r="F34" s="72">
         <v>2</v>
       </c>
-      <c r="G34" s="68"/>
+      <c r="F34" s="68"/>
+      <c r="G34" s="72">
+        <v>1</v>
+      </c>
       <c r="H34" s="72">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I34" s="69"/>
       <c r="J34" s="67"/>
@@ -4487,41 +4485,47 @@
     </row>
     <row r="35" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A35" s="64" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="B35" s="65" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C35" s="66" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="D35" s="127" t="s">
-        <v>148</v>
-      </c>
-      <c r="E35" s="70">
-        <v>2</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="E35" s="67"/>
       <c r="F35" s="68"/>
       <c r="G35" s="72">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H35" s="72">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I35" s="69"/>
-      <c r="J35" s="67"/>
-      <c r="K35" s="68"/>
-      <c r="L35" s="68"/>
-      <c r="M35" s="68"/>
-      <c r="N35" s="73"/>
+      <c r="J35" s="70">
+        <v>1</v>
+      </c>
+      <c r="K35" s="71" t="s">
+        <v>17</v>
+      </c>
+      <c r="L35" s="72">
+        <v>1</v>
+      </c>
+      <c r="M35" s="71" t="s">
+        <v>18</v>
+      </c>
+      <c r="N35" s="72"/>
       <c r="O35" s="72"/>
-      <c r="P35" s="73"/>
+      <c r="P35" s="72"/>
       <c r="Q35" s="72"/>
-      <c r="R35" s="73"/>
+      <c r="R35" s="72"/>
     </row>
     <row r="36" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A36" s="64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B36" s="65" t="s">
         <v>52</v>
@@ -4530,13 +4534,13 @@
         <v>10</v>
       </c>
       <c r="D36" s="127" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E36" s="67"/>
-      <c r="F36" s="68"/>
-      <c r="G36" s="72">
+      <c r="F36" s="72">
         <v>2</v>
       </c>
+      <c r="G36" s="68"/>
       <c r="H36" s="72">
         <v>1</v>
       </c>
@@ -4561,7 +4565,7 @@
     </row>
     <row r="37" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A37" s="64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B37" s="65" t="s">
         <v>53</v>
@@ -4580,18 +4584,20 @@
       <c r="H37" s="72">
         <v>1</v>
       </c>
-      <c r="I37" s="69"/>
+      <c r="I37" s="128">
+        <v>1</v>
+      </c>
       <c r="J37" s="70">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K37" s="71" t="s">
         <v>17</v>
       </c>
       <c r="L37" s="72">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M37" s="71" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="N37" s="72"/>
       <c r="O37" s="72"/>
@@ -4601,7 +4607,7 @@
     </row>
     <row r="38" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A38" s="64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B38" s="65" t="s">
         <v>54</v>
@@ -4610,12 +4616,12 @@
         <v>10</v>
       </c>
       <c r="D38" s="127" t="s">
-        <v>152</v>
-      </c>
-      <c r="E38" s="67"/>
-      <c r="F38" s="72">
+        <v>151</v>
+      </c>
+      <c r="E38" s="70">
         <v>2</v>
       </c>
+      <c r="F38" s="68"/>
       <c r="G38" s="68"/>
       <c r="H38" s="72">
         <v>1</v>
@@ -4624,16 +4630,16 @@
         <v>1</v>
       </c>
       <c r="J38" s="70">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K38" s="71" t="s">
+        <v>33</v>
+      </c>
+      <c r="L38" s="72">
+        <v>1</v>
+      </c>
+      <c r="M38" s="71" t="s">
         <v>17</v>
-      </c>
-      <c r="L38" s="72">
-        <v>2</v>
-      </c>
-      <c r="M38" s="71" t="s">
-        <v>33</v>
       </c>
       <c r="N38" s="72"/>
       <c r="O38" s="72"/>
@@ -4643,7 +4649,7 @@
     </row>
     <row r="39" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A39" s="64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B39" s="65" t="s">
         <v>55</v>
@@ -4652,27 +4658,23 @@
         <v>10</v>
       </c>
       <c r="D39" s="127" t="s">
-        <v>153</v>
-      </c>
-      <c r="E39" s="70">
-        <v>2</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="E39" s="67"/>
       <c r="F39" s="68"/>
       <c r="G39" s="68"/>
-      <c r="H39" s="72">
-        <v>1</v>
-      </c>
+      <c r="H39" s="68"/>
       <c r="I39" s="128">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J39" s="70">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K39" s="71" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="L39" s="72">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M39" s="71" t="s">
         <v>17</v>
@@ -4685,7 +4687,7 @@
     </row>
     <row r="40" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A40" s="64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B40" s="65" t="s">
         <v>56</v>
@@ -4694,124 +4696,124 @@
         <v>10</v>
       </c>
       <c r="D40" s="127" t="s">
-        <v>154</v>
-      </c>
-      <c r="E40" s="67"/>
+        <v>153</v>
+      </c>
+      <c r="E40" s="70">
+        <v>2</v>
+      </c>
       <c r="F40" s="68"/>
-      <c r="G40" s="68"/>
+      <c r="G40" s="72">
+        <v>2</v>
+      </c>
       <c r="H40" s="68"/>
       <c r="I40" s="128">
-        <v>3</v>
-      </c>
-      <c r="J40" s="70">
-        <v>2</v>
-      </c>
-      <c r="K40" s="71" t="s">
-        <v>14</v>
-      </c>
-      <c r="L40" s="72">
-        <v>2</v>
-      </c>
-      <c r="M40" s="71" t="s">
-        <v>17</v>
-      </c>
-      <c r="N40" s="72"/>
-      <c r="O40" s="72"/>
-      <c r="P40" s="72"/>
-      <c r="Q40" s="72"/>
-      <c r="R40" s="72"/>
+        <v>1</v>
+      </c>
+      <c r="J40" s="70"/>
+      <c r="K40" s="71"/>
+      <c r="L40" s="129"/>
+      <c r="M40" s="68"/>
+      <c r="N40" s="129" t="s">
+        <v>126</v>
+      </c>
+      <c r="O40" s="72">
+        <v>1</v>
+      </c>
+      <c r="P40" s="73" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q40" s="72">
+        <v>1</v>
+      </c>
+      <c r="R40" s="73" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="41" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A41" s="64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B41" s="65" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C41" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D41" s="127" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E41" s="70">
         <v>2</v>
       </c>
-      <c r="F41" s="68"/>
+      <c r="F41" s="72">
+        <v>2</v>
+      </c>
       <c r="G41" s="72">
         <v>2</v>
       </c>
       <c r="H41" s="68"/>
-      <c r="I41" s="128">
-        <v>1</v>
-      </c>
+      <c r="I41" s="69"/>
       <c r="J41" s="70"/>
       <c r="K41" s="71"/>
       <c r="L41" s="129"/>
       <c r="M41" s="68"/>
       <c r="N41" s="129" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O41" s="72">
         <v>1</v>
       </c>
       <c r="P41" s="73" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q41" s="72">
         <v>1</v>
       </c>
       <c r="R41" s="73" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A42" s="64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B42" s="65" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C42" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D42" s="127" t="s">
-        <v>156</v>
-      </c>
-      <c r="E42" s="70">
-        <v>2</v>
-      </c>
-      <c r="F42" s="72">
-        <v>2</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="E42" s="67"/>
+      <c r="F42" s="68"/>
       <c r="G42" s="72">
-        <v>2</v>
-      </c>
-      <c r="H42" s="68"/>
-      <c r="I42" s="69"/>
-      <c r="J42" s="70"/>
-      <c r="K42" s="71"/>
-      <c r="L42" s="129"/>
+        <v>1</v>
+      </c>
+      <c r="H42" s="72">
+        <v>1</v>
+      </c>
+      <c r="I42" s="128">
+        <v>1</v>
+      </c>
+      <c r="J42" s="70">
+        <v>3</v>
+      </c>
+      <c r="K42" s="71" t="s">
+        <v>32</v>
+      </c>
+      <c r="L42" s="68"/>
       <c r="M42" s="68"/>
-      <c r="N42" s="129" t="s">
-        <v>127</v>
-      </c>
-      <c r="O42" s="72">
-        <v>1</v>
-      </c>
-      <c r="P42" s="73" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q42" s="72">
-        <v>1</v>
-      </c>
-      <c r="R42" s="73" t="s">
-        <v>7</v>
-      </c>
+      <c r="N42" s="73"/>
+      <c r="O42" s="72"/>
+      <c r="P42" s="73"/>
+      <c r="Q42" s="72"/>
+      <c r="R42" s="73"/>
     </row>
     <row r="43" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A43" s="64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B43" s="65" t="s">
         <v>61</v>
@@ -4820,13 +4822,13 @@
         <v>10</v>
       </c>
       <c r="D43" s="127" t="s">
-        <v>157</v>
+        <v>215</v>
       </c>
       <c r="E43" s="67"/>
-      <c r="F43" s="68"/>
-      <c r="G43" s="72">
-        <v>1</v>
-      </c>
+      <c r="F43" s="72">
+        <v>1</v>
+      </c>
+      <c r="G43" s="68"/>
       <c r="H43" s="72">
         <v>1</v>
       </c>
@@ -4836,7 +4838,7 @@
       <c r="J43" s="70">
         <v>3</v>
       </c>
-      <c r="K43" s="71" t="s">
+      <c r="K43" s="76" t="s">
         <v>33</v>
       </c>
       <c r="L43" s="68"/>
@@ -4849,33 +4851,31 @@
     </row>
     <row r="44" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A44" s="64" t="s">
-        <v>51</v>
-      </c>
-      <c r="B44" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="B44" s="77" t="s">
         <v>62</v>
       </c>
       <c r="C44" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D44" s="127" t="s">
-        <v>217</v>
-      </c>
-      <c r="E44" s="67"/>
-      <c r="F44" s="72">
-        <v>1</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="E44" s="70">
+        <v>4</v>
+      </c>
+      <c r="F44" s="68"/>
       <c r="G44" s="68"/>
-      <c r="H44" s="72">
-        <v>1</v>
-      </c>
+      <c r="H44" s="68"/>
       <c r="I44" s="128">
         <v>1</v>
       </c>
       <c r="J44" s="70">
         <v>3</v>
       </c>
-      <c r="K44" s="76" t="s">
-        <v>34</v>
+      <c r="K44" s="71" t="s">
+        <v>11</v>
       </c>
       <c r="L44" s="68"/>
       <c r="M44" s="68"/>
@@ -4887,7 +4887,7 @@
     </row>
     <row r="45" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A45" s="64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B45" s="77" t="s">
         <v>63</v>
@@ -4896,7 +4896,7 @@
         <v>10</v>
       </c>
       <c r="D45" s="127" t="s">
-        <v>211</v>
+        <v>156</v>
       </c>
       <c r="E45" s="70">
         <v>4</v>
@@ -4904,14 +4904,12 @@
       <c r="F45" s="68"/>
       <c r="G45" s="68"/>
       <c r="H45" s="68"/>
-      <c r="I45" s="128">
-        <v>1</v>
-      </c>
+      <c r="I45" s="69"/>
       <c r="J45" s="70">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K45" s="71" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="L45" s="68"/>
       <c r="M45" s="68"/>
@@ -4923,7 +4921,7 @@
     </row>
     <row r="46" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A46" s="64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B46" s="77" t="s">
         <v>64</v>
@@ -4932,13 +4930,15 @@
         <v>10</v>
       </c>
       <c r="D46" s="127" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E46" s="70">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F46" s="68"/>
-      <c r="G46" s="68"/>
+      <c r="G46" s="72">
+        <v>2</v>
+      </c>
       <c r="H46" s="68"/>
       <c r="I46" s="69"/>
       <c r="J46" s="70">
@@ -4947,57 +4947,57 @@
       <c r="K46" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="L46" s="68"/>
-      <c r="M46" s="68"/>
-      <c r="N46" s="73"/>
+      <c r="L46" s="72">
+        <v>1</v>
+      </c>
+      <c r="M46" s="71" t="s">
+        <v>17</v>
+      </c>
+      <c r="N46" s="72"/>
       <c r="O46" s="72"/>
-      <c r="P46" s="73"/>
+      <c r="P46" s="72"/>
       <c r="Q46" s="72"/>
-      <c r="R46" s="73"/>
+      <c r="R46" s="72"/>
     </row>
     <row r="47" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A47" s="64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B47" s="77" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C47" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D47" s="127" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E47" s="70">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F47" s="68"/>
       <c r="G47" s="72">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H47" s="68"/>
-      <c r="I47" s="69"/>
-      <c r="J47" s="70">
-        <v>2</v>
-      </c>
+      <c r="I47" s="128">
+        <v>6</v>
+      </c>
+      <c r="J47" s="67"/>
       <c r="K47" s="71" t="s">
-        <v>14</v>
-      </c>
-      <c r="L47" s="72">
-        <v>1</v>
-      </c>
-      <c r="M47" s="71" t="s">
-        <v>17</v>
-      </c>
-      <c r="N47" s="72"/>
+        <v>65</v>
+      </c>
+      <c r="L47" s="68"/>
+      <c r="M47" s="68"/>
+      <c r="N47" s="73"/>
       <c r="O47" s="72"/>
-      <c r="P47" s="72"/>
+      <c r="P47" s="73"/>
       <c r="Q47" s="72"/>
-      <c r="R47" s="72"/>
+      <c r="R47" s="73"/>
     </row>
     <row r="48" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A48" s="64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B48" s="77" t="s">
         <v>67</v>
@@ -5006,12 +5006,12 @@
         <v>10</v>
       </c>
       <c r="D48" s="127" t="s">
-        <v>160</v>
-      </c>
-      <c r="E48" s="70">
-        <v>12</v>
-      </c>
-      <c r="F48" s="68"/>
+        <v>216</v>
+      </c>
+      <c r="E48" s="67"/>
+      <c r="F48" s="72">
+        <v>10</v>
+      </c>
       <c r="G48" s="72">
         <v>10</v>
       </c>
@@ -5021,7 +5021,7 @@
       </c>
       <c r="J48" s="67"/>
       <c r="K48" s="71" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L48" s="68"/>
       <c r="M48" s="68"/>
@@ -5033,31 +5033,31 @@
     </row>
     <row r="49" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A49" s="64" t="s">
-        <v>51</v>
-      </c>
-      <c r="B49" s="77" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" s="65" t="s">
         <v>68</v>
       </c>
       <c r="C49" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D49" s="127" t="s">
-        <v>218</v>
-      </c>
-      <c r="E49" s="67"/>
+        <v>159</v>
+      </c>
+      <c r="E49" s="70">
+        <v>12</v>
+      </c>
       <c r="F49" s="72">
         <v>10</v>
       </c>
-      <c r="G49" s="72">
-        <v>10</v>
-      </c>
+      <c r="G49" s="68"/>
       <c r="H49" s="68"/>
       <c r="I49" s="128">
         <v>6</v>
       </c>
       <c r="J49" s="67"/>
       <c r="K49" s="71" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L49" s="68"/>
       <c r="M49" s="68"/>
@@ -5069,31 +5069,31 @@
     </row>
     <row r="50" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A50" s="64" t="s">
-        <v>51</v>
-      </c>
-      <c r="B50" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="77" t="s">
         <v>69</v>
       </c>
       <c r="C50" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D50" s="127" t="s">
-        <v>161</v>
-      </c>
-      <c r="E50" s="70">
-        <v>12</v>
-      </c>
-      <c r="F50" s="72">
+        <v>217</v>
+      </c>
+      <c r="E50" s="67"/>
+      <c r="F50" s="68"/>
+      <c r="G50" s="72">
         <v>10</v>
       </c>
-      <c r="G50" s="68"/>
-      <c r="H50" s="68"/>
+      <c r="H50" s="72">
+        <v>8</v>
+      </c>
       <c r="I50" s="128">
         <v>6</v>
       </c>
       <c r="J50" s="67"/>
       <c r="K50" s="71" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L50" s="68"/>
       <c r="M50" s="68"/>
@@ -5105,22 +5105,22 @@
     </row>
     <row r="51" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A51" s="64" t="s">
-        <v>51</v>
-      </c>
-      <c r="B51" s="77" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" s="65" t="s">
         <v>70</v>
       </c>
       <c r="C51" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D51" s="127" t="s">
-        <v>219</v>
+        <v>160</v>
       </c>
       <c r="E51" s="67"/>
-      <c r="F51" s="68"/>
-      <c r="G51" s="72">
+      <c r="F51" s="72">
         <v>10</v>
       </c>
+      <c r="G51" s="68"/>
       <c r="H51" s="72">
         <v>8</v>
       </c>
@@ -5129,7 +5129,7 @@
       </c>
       <c r="J51" s="67"/>
       <c r="K51" s="71" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L51" s="68"/>
       <c r="M51" s="68"/>
@@ -5141,21 +5141,21 @@
     </row>
     <row r="52" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A52" s="64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52" s="65" t="s">
-        <v>71</v>
+        <v>221</v>
       </c>
       <c r="C52" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D52" s="127" t="s">
-        <v>162</v>
-      </c>
-      <c r="E52" s="67"/>
-      <c r="F52" s="72">
-        <v>10</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="E52" s="67">
+        <v>12</v>
+      </c>
+      <c r="F52" s="72"/>
       <c r="G52" s="68"/>
       <c r="H52" s="72">
         <v>8</v>
@@ -5165,7 +5165,7 @@
       </c>
       <c r="J52" s="67"/>
       <c r="K52" s="71" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L52" s="68"/>
       <c r="M52" s="68"/>
@@ -5177,16 +5177,16 @@
     </row>
     <row r="53" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A53" s="64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" s="65" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C53" s="66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D53" s="127" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E53" s="70">
         <v>2</v>
@@ -5217,16 +5217,16 @@
     </row>
     <row r="54" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A54" s="64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B54" s="65" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C54" s="66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D54" s="127" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E54" s="67"/>
       <c r="F54" s="68"/>
@@ -5245,7 +5245,7 @@
         <v>1</v>
       </c>
       <c r="M54" s="71" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N54" s="72"/>
       <c r="O54" s="72"/>
@@ -5255,16 +5255,16 @@
     </row>
     <row r="55" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A55" s="64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B55" s="65" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C55" s="66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D55" s="127" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E55" s="67"/>
       <c r="F55" s="72">
@@ -5283,7 +5283,7 @@
         <v>1</v>
       </c>
       <c r="M55" s="71" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N55" s="72"/>
       <c r="O55" s="72"/>
@@ -5293,16 +5293,16 @@
     </row>
     <row r="56" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A56" s="64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B56" s="65" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C56" s="66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D56" s="127" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E56" s="70">
         <v>2</v>
@@ -5322,33 +5322,33 @@
       <c r="L56" s="72"/>
       <c r="M56" s="68"/>
       <c r="N56" s="72" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O56" s="72">
         <v>1</v>
       </c>
       <c r="P56" s="73" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q56" s="72">
         <v>1</v>
       </c>
       <c r="R56" s="73" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A57" s="64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B57" s="65" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C57" s="66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D57" s="127" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E57" s="67"/>
       <c r="F57" s="68"/>
@@ -5373,16 +5373,16 @@
     </row>
     <row r="58" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A58" s="64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B58" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C58" s="66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D58" s="127" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E58" s="67"/>
       <c r="F58" s="72">
@@ -5413,19 +5413,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:D58">
-    <cfRule type="containsText" dxfId="7" priority="1" stopIfTrue="1" operator="containsText" text="3+">
+    <cfRule type="containsText" dxfId="3" priority="1" stopIfTrue="1" operator="containsText" text="3+">
       <formula>NOT(ISERROR(FIND(UPPER("3+"),UPPER(C1))))</formula>
       <formula>"3+"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" stopIfTrue="1" operator="containsText" text="1+">
+    <cfRule type="containsText" dxfId="2" priority="2" stopIfTrue="1" operator="containsText" text="1+">
       <formula>NOT(ISERROR(FIND(UPPER("1+"),UPPER(C1))))</formula>
       <formula>"1+"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" stopIfTrue="1" operator="containsText" text="1-4">
+    <cfRule type="containsText" dxfId="1" priority="3" stopIfTrue="1" operator="containsText" text="1-4">
       <formula>NOT(ISERROR(FIND(UPPER("1-4"),UPPER(C1))))</formula>
       <formula>"1-4"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" stopIfTrue="1" operator="containsText" text="1-2">
+    <cfRule type="containsText" dxfId="0" priority="4" stopIfTrue="1" operator="containsText" text="1-2">
       <formula>NOT(ISERROR(FIND(UPPER("1-2"),UPPER(C1))))</formula>
       <formula>"1-2"</formula>
     </cfRule>
@@ -5442,8 +5442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IK16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5476,60 +5476,60 @@
         <v>2</v>
       </c>
       <c r="D1" s="135" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E1" s="107" t="s">
+        <v>172</v>
+      </c>
+      <c r="F1" s="107" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1" s="107" t="s">
         <v>174</v>
       </c>
-      <c r="F1" s="107" t="s">
+      <c r="H1" s="107" t="s">
         <v>175</v>
       </c>
-      <c r="G1" s="107" t="s">
-        <v>176</v>
-      </c>
-      <c r="H1" s="107" t="s">
-        <v>177</v>
-      </c>
       <c r="I1" s="111" t="s">
+        <v>164</v>
+      </c>
+      <c r="J1" s="114" t="s">
+        <v>165</v>
+      </c>
+      <c r="K1" s="114" t="s">
         <v>166</v>
       </c>
-      <c r="J1" s="114" t="s">
+      <c r="L1" s="114" t="s">
         <v>167</v>
       </c>
-      <c r="K1" s="114" t="s">
+      <c r="M1" s="112" t="s">
+        <v>126</v>
+      </c>
+      <c r="N1" s="112" t="s">
         <v>168</v>
       </c>
-      <c r="L1" s="114" t="s">
+      <c r="O1" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="M1" s="112" t="s">
-        <v>127</v>
-      </c>
-      <c r="N1" s="112" t="s">
+      <c r="P1" s="112" t="s">
         <v>170</v>
       </c>
-      <c r="O1" s="112" t="s">
+      <c r="Q1" s="112" t="s">
         <v>171</v>
-      </c>
-      <c r="P1" s="112" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q1" s="112" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" s="79" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C2" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="134" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E2" s="81"/>
       <c r="F2" s="82"/>
@@ -5540,13 +5540,13 @@
       <c r="K2" s="86"/>
       <c r="L2" s="82"/>
       <c r="M2" s="86" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N2" s="86">
         <v>2</v>
       </c>
       <c r="O2" s="87" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P2" s="86">
         <v>1</v>
@@ -5785,16 +5785,16 @@
     </row>
     <row r="3" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="79" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C3" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="134" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E3" s="84">
         <v>1</v>
@@ -5813,13 +5813,13 @@
       <c r="K3" s="86"/>
       <c r="L3" s="82"/>
       <c r="M3" s="86" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N3" s="86">
         <v>1</v>
       </c>
       <c r="O3" s="87" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P3" s="86">
         <v>1</v>
@@ -6058,16 +6058,16 @@
     </row>
     <row r="4" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" s="79" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C4" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="134" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E4" s="84">
         <v>1</v>
@@ -6086,13 +6086,13 @@
       <c r="K4" s="86"/>
       <c r="L4" s="82"/>
       <c r="M4" s="86" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N4" s="86">
         <v>1</v>
       </c>
       <c r="O4" s="87" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P4" s="86">
         <v>1</v>
@@ -6331,16 +6331,16 @@
     </row>
     <row r="5" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="78" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="79" t="s">
         <v>79</v>
-      </c>
-      <c r="B5" s="79" t="s">
-        <v>80</v>
       </c>
       <c r="C5" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="134" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E5" s="84">
         <v>1</v>
@@ -6355,13 +6355,13 @@
       <c r="K5" s="86"/>
       <c r="L5" s="82"/>
       <c r="M5" s="86" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N5" s="86">
         <v>1</v>
       </c>
       <c r="O5" s="87" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P5" s="86">
         <v>2</v>
@@ -6600,16 +6600,16 @@
     </row>
     <row r="6" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="79" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="134" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E6" s="81"/>
       <c r="F6" s="82"/>
@@ -6859,16 +6859,16 @@
     </row>
     <row r="7" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" s="79" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C7" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="134" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E7" s="84">
         <v>2</v>
@@ -6883,7 +6883,7 @@
       <c r="K7" s="86"/>
       <c r="L7" s="82"/>
       <c r="M7" s="86" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N7" s="86">
         <v>1</v>
@@ -7128,16 +7128,16 @@
     </row>
     <row r="8" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" s="79" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C8" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="134" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E8" s="81"/>
       <c r="F8" s="82"/>
@@ -7387,16 +7387,16 @@
     </row>
     <row r="9" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B9" s="79" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C9" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="138" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E9" s="84">
         <v>3</v>
@@ -7411,7 +7411,7 @@
       <c r="K9" s="86"/>
       <c r="L9" s="82"/>
       <c r="M9" s="86" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N9" s="86">
         <v>1</v>
@@ -7423,7 +7423,7 @@
         <v>1</v>
       </c>
       <c r="Q9" s="87" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R9" s="88"/>
       <c r="S9" s="88"/>
@@ -7656,16 +7656,16 @@
     </row>
     <row r="10" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B10" s="79" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="134" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E10" s="84">
         <v>1</v>
@@ -7679,7 +7679,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="90" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="K10" s="86"/>
       <c r="L10" s="85"/>
@@ -7919,16 +7919,16 @@
     </row>
     <row r="11" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B11" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C11" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="134" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E11" s="84">
         <v>2</v>
@@ -8186,16 +8186,16 @@
     </row>
     <row r="12" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B12" s="79" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C12" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="134" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E12" s="84">
         <v>2</v>
@@ -8210,19 +8210,19 @@
       <c r="K12" s="86"/>
       <c r="L12" s="82"/>
       <c r="M12" s="86" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N12" s="86">
         <v>1</v>
       </c>
       <c r="O12" s="87" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P12" s="86">
         <v>1</v>
       </c>
       <c r="Q12" s="87" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R12" s="88"/>
       <c r="S12" s="88"/>
@@ -8455,16 +8455,16 @@
     </row>
     <row r="13" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B13" s="92" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C13" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="134" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E13" s="93"/>
       <c r="F13" s="82"/>
@@ -8472,7 +8472,7 @@
       <c r="H13" s="83"/>
       <c r="I13" s="84"/>
       <c r="J13" s="85" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K13" s="87"/>
       <c r="L13" s="94"/>
@@ -8712,16 +8712,16 @@
     </row>
     <row r="14" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B14" s="92" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C14" s="80" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14" s="134" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E14" s="84">
         <v>1</v>
@@ -8736,13 +8736,13 @@
       <c r="K14" s="86"/>
       <c r="L14" s="85"/>
       <c r="M14" s="86" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N14" s="86">
         <v>1</v>
       </c>
       <c r="O14" s="86" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P14" s="86">
         <v>1</v>
@@ -8981,16 +8981,16 @@
     </row>
     <row r="15" spans="1:245" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B15" s="92" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C15" s="80" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D15" s="134" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E15" s="84">
         <v>2</v>
@@ -9005,7 +9005,7 @@
       <c r="K15" s="86"/>
       <c r="L15" s="94"/>
       <c r="M15" s="86" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N15" s="86">
         <v>1</v>
@@ -9017,7 +9017,7 @@
         <v>1</v>
       </c>
       <c r="Q15" s="87" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R15" s="88"/>
       <c r="S15" s="88"/>
@@ -9250,16 +9250,16 @@
     </row>
     <row r="16" spans="1:245" s="106" customFormat="1" ht="15.75" customHeight="1">
       <c r="A16" s="97" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B16" s="98" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C16" s="99" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D16" s="136" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E16" s="100">
         <v>1</v>
@@ -9517,19 +9517,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:D16">
-    <cfRule type="containsText" dxfId="3" priority="1" stopIfTrue="1" operator="containsText" text="3+">
+    <cfRule type="containsText" dxfId="7" priority="1" stopIfTrue="1" operator="containsText" text="3+">
       <formula>NOT(ISERROR(FIND(UPPER("3+"),UPPER(C2))))</formula>
       <formula>"3+"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" stopIfTrue="1" operator="containsText" text="1+">
+    <cfRule type="containsText" dxfId="6" priority="2" stopIfTrue="1" operator="containsText" text="1+">
       <formula>NOT(ISERROR(FIND(UPPER("1+"),UPPER(C2))))</formula>
       <formula>"1+"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" stopIfTrue="1" operator="containsText" text="1-4">
+    <cfRule type="containsText" dxfId="5" priority="3" stopIfTrue="1" operator="containsText" text="1-4">
       <formula>NOT(ISERROR(FIND(UPPER("1-4"),UPPER(C2))))</formula>
       <formula>"1-4"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="4" stopIfTrue="1" operator="containsText" text="1-2">
+    <cfRule type="containsText" dxfId="4" priority="4" stopIfTrue="1" operator="containsText" text="1-2">
       <formula>NOT(ISERROR(FIND(UPPER("1-2"),UPPER(C2))))</formula>
       <formula>"1-2"</formula>
     </cfRule>
@@ -9561,22 +9561,22 @@
         <v>0</v>
       </c>
       <c r="C1" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="27" t="s">
         <v>96</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>97</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="6"/>
@@ -9586,10 +9586,10 @@
         <v>17</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D3" s="29"/>
       <c r="E3" s="6"/>
@@ -9599,23 +9599,23 @@
         <v>14</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D4" s="29"/>
       <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>100</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>101</v>
       </c>
       <c r="D5" s="29"/>
       <c r="E5" s="6"/>
@@ -9625,20 +9625,20 @@
         <v>18</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D6" s="29"/>
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="6"/>
@@ -9646,10 +9646,10 @@
     </row>
     <row r="8" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="6"/>
@@ -9657,10 +9657,10 @@
     </row>
     <row r="9" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C9" s="29"/>
       <c r="D9" s="6"/>
@@ -9668,10 +9668,10 @@
     </row>
     <row r="10" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C10" s="29"/>
       <c r="D10" s="6"/>
@@ -9679,10 +9679,10 @@
     </row>
     <row r="11" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C11" s="29"/>
       <c r="D11" s="6"/>
@@ -9690,10 +9690,10 @@
     </row>
     <row r="12" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="6"/>
@@ -9701,10 +9701,10 @@
     </row>
     <row r="13" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C13" s="29"/>
       <c r="D13" s="6"/>
@@ -9712,10 +9712,10 @@
     </row>
     <row r="14" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C14" s="29"/>
       <c r="D14" s="6"/>
@@ -9723,10 +9723,10 @@
     </row>
     <row r="15" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C15" s="29"/>
       <c r="D15" s="6"/>
@@ -9734,10 +9734,10 @@
     </row>
     <row r="16" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C16" s="29"/>
       <c r="D16" s="6"/>
@@ -9745,10 +9745,10 @@
     </row>
     <row r="17" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C17" s="29"/>
       <c r="D17" s="6"/>
@@ -9756,10 +9756,10 @@
     </row>
     <row r="18" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A18" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C18" s="29"/>
       <c r="D18" s="6"/>
@@ -9767,10 +9767,10 @@
     </row>
     <row r="19" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C19" s="29"/>
       <c r="D19" s="6"/>
@@ -9781,10 +9781,10 @@
         <v>11</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D20" s="32"/>
       <c r="E20" s="6"/>
@@ -9794,10 +9794,10 @@
         <v>7</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>106</v>
       </c>
       <c r="D21" s="34"/>
       <c r="E21" s="6"/>
@@ -9807,10 +9807,10 @@
         <v>6</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D22" s="29"/>
       <c r="E22" s="6"/>
@@ -9820,10 +9820,10 @@
         <v>5</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D23" s="29"/>
       <c r="E23" s="6"/>
@@ -9833,10 +9833,10 @@
         <v>3</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D24" s="29"/>
       <c r="E24" s="6"/>
@@ -9846,10 +9846,10 @@
         <v>4</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D25" s="29"/>
       <c r="E25" s="6"/>
@@ -9891,24 +9891,24 @@
   <sheetData>
     <row r="1" spans="1:18" ht="17.100000000000001" customHeight="1">
       <c r="A1" s="144" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B1" s="141"/>
       <c r="C1" s="140" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D1" s="145"/>
       <c r="E1" s="141"/>
       <c r="F1" s="140" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G1" s="141"/>
       <c r="H1" s="140" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I1" s="141"/>
       <c r="J1" s="140" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K1" s="141"/>
       <c r="L1" s="29"/>
@@ -9927,37 +9927,37 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>119</v>
       </c>
       <c r="N2" s="37"/>
       <c r="O2" s="6"/>
@@ -10126,11 +10126,11 @@
       </c>
       <c r="D7" s="10">
         <f>SUMIF(Junk!$C1:$C58,"1+",Junk!E1:E58)</f>
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="E7" s="39">
         <f>SUM(Junk!E1:E58)</f>
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="F7" s="8">
         <v>1</v>
@@ -10176,15 +10176,15 @@
       </c>
       <c r="C8" s="14">
         <f>COUNTA(Junk!F2:F58)</f>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="12">
         <f>SUMIF(Junk!$C1:$C58,"1+",Junk!F1:F58)</f>
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E8" s="43">
         <f>SUM(Junk!F1:F58)</f>
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F8" s="14">
         <v>1</v>
@@ -10208,7 +10208,7 @@
       </c>
       <c r="L8" s="14">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M8" s="12" t="e">
         <f t="shared" si="1"/>
@@ -10285,15 +10285,15 @@
       </c>
       <c r="C10" s="14">
         <f>COUNTA(Junk!H2:H58)</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10" s="12">
         <f>SUMIF(Junk!$C1:$C58,"1+",Junk!H1:H58)</f>
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E10" s="43">
         <f>SUM(Junk!H1:H58)</f>
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="F10" s="14">
         <v>1</v>
@@ -10317,7 +10317,7 @@
       </c>
       <c r="L10" s="14">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M10" s="43" t="e">
         <f t="shared" si="1"/>
@@ -10340,15 +10340,15 @@
       </c>
       <c r="C11" s="21">
         <f>COUNTA(Junk!I2:I58)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D11" s="22">
         <f>SUMIF(Junk!$C1:$C58,"1+",Junk!I1:I58)</f>
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E11" s="45">
         <f>SUM(Junk!I1:I58)</f>
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F11" s="21">
         <v>1</v>
@@ -10372,7 +10372,7 @@
       </c>
       <c r="L11" s="21">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M11" s="45" t="e">
         <f t="shared" si="1"/>
@@ -10409,17 +10409,17 @@
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" s="53" t="s">
         <v>120</v>
       </c>
-      <c r="E13" s="53" t="s">
+      <c r="F13" s="140" t="s">
         <v>121</v>
-      </c>
-      <c r="F13" s="140" t="s">
-        <v>122</v>
       </c>
       <c r="G13" s="141"/>
       <c r="H13" s="142" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I13" s="143"/>
       <c r="J13" s="42"/>
@@ -10437,16 +10437,16 @@
         <v>3</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="54">
         <f t="shared" ref="D14:E17" si="2">SUM(D$7:D$10)/D7</f>
-        <v>3.1025641025641026</v>
+        <v>2.9318181818181817</v>
       </c>
       <c r="E14" s="55">
         <f t="shared" si="2"/>
-        <v>3.1122448979591835</v>
+        <v>2.9722222222222223</v>
       </c>
       <c r="F14" s="56">
         <f>F7/C7</f>
@@ -10462,7 +10462,7 @@
       </c>
       <c r="I14" s="58">
         <f>I7/E7</f>
-        <v>5.1020408163265307E-2</v>
+        <v>4.6296296296296294E-2</v>
       </c>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
@@ -10479,20 +10479,20 @@
         <v>4</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="54">
         <f t="shared" si="2"/>
-        <v>3.903225806451613</v>
+        <v>4.3</v>
       </c>
       <c r="E15" s="55">
         <f t="shared" si="2"/>
-        <v>3.9610389610389611</v>
+        <v>4.28</v>
       </c>
       <c r="F15" s="56">
         <f>F8/C8</f>
-        <v>3.5714285714285712E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
       <c r="G15" s="57">
         <f>G8/E8</f>
@@ -10521,16 +10521,16 @@
         <v>5</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="54">
         <f t="shared" si="2"/>
-        <v>3.8412698412698414</v>
+        <v>4.0952380952380949</v>
       </c>
       <c r="E16" s="55">
         <f t="shared" si="2"/>
-        <v>3.8607594936708862</v>
+        <v>4.0632911392405067</v>
       </c>
       <c r="F16" s="56">
         <f>F9/C9</f>
@@ -10563,20 +10563,20 @@
         <v>6</v>
       </c>
       <c r="B17" s="45" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C17" s="32"/>
       <c r="D17" s="59">
         <f t="shared" si="2"/>
-        <v>6.2051282051282053</v>
+        <v>5.4893617021276597</v>
       </c>
       <c r="E17" s="60">
         <f t="shared" si="2"/>
-        <v>5.9803921568627452</v>
+        <v>5.4406779661016946</v>
       </c>
       <c r="F17" s="61">
         <f>F10/C10</f>
-        <v>3.8461538461538464E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
       <c r="G17" s="62">
         <f>G10/E10</f>
@@ -10615,7 +10615,7 @@
       <c r="L18" s="6"/>
       <c r="M18" s="11"/>
       <c r="N18" s="63" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="O18" s="6"/>
       <c r="P18" s="4" t="s">
@@ -10648,7 +10648,7 @@
       </c>
       <c r="P19" s="4">
         <f>COUNTIFS(Junk!E1:E58,"&gt;0",Junk!F1:F58,"&gt;0")</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q19" s="4">
         <f>COUNTIFS(Junk!E1:E58,"&gt;0",Junk!G1:G58,"&gt;0")</f>
@@ -10656,7 +10656,7 @@
       </c>
       <c r="R19" s="4">
         <f>COUNTIFS(Junk!E1:E58,"&gt;0",Junk!H1:H58,"&gt;0")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="17.100000000000001" customHeight="1">

</xml_diff>

<commit_message>
Some snark writing and tweaking.
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="16440"/>
@@ -12,7 +12,7 @@
     <sheet name="Primitives" sheetId="2" r:id="rId3"/>
     <sheet name="Stats" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -64,9 +64,6 @@
     <t>capacity</t>
   </si>
   <si>
-    <t>Sack of Door Knobs</t>
-  </si>
-  <si>
     <t>Rusty Bicycle Chain</t>
   </si>
   <si>
@@ -130,9 +127,6 @@
     <t>take glass</t>
   </si>
   <si>
-    <t>Shack with Nice Curtains</t>
-  </si>
-  <si>
     <t>Perfectly Folded Laundry</t>
   </si>
   <si>
@@ -412,9 +406,6 @@
     <t>"Nothing says 'scram!' like a man with a flail."</t>
   </si>
   <si>
-    <t>"Woah. Wonder what happened here."</t>
-  </si>
-  <si>
     <t>"A distraction is as good as a stab."</t>
   </si>
   <si>
@@ -433,9 +424,6 @@
     <t>"Don't mess with vandals who can knit."</t>
   </si>
   <si>
-    <t>"The gift that keeps on giving. And distracting my enemies."</t>
-  </si>
-  <si>
     <t>"Why do I feel the need to swing on something?"</t>
   </si>
   <si>
@@ -496,9 +484,6 @@
     <t>"I wonder how cyborgs worked during the Steampunk Age."</t>
   </si>
   <si>
-    <t>"Now with more  disease!"</t>
-  </si>
-  <si>
     <t>"Victory is mine. And now everyone knows it."</t>
   </si>
   <si>
@@ -508,9 +493,6 @@
     <t>"Great for traversing those Papershred Hills!"</t>
   </si>
   <si>
-    <t>"Where's my allen wrench?"</t>
-  </si>
-  <si>
     <t>bonus1_num</t>
   </si>
   <si>
@@ -577,18 +559,9 @@
     <t>"A friend in need is a friend without trash."</t>
   </si>
   <si>
-    <t>"None may know the hour of my arrival.</t>
-  </si>
-  <si>
     <t>"I eat dirt like you for breakfast!"</t>
   </si>
   <si>
-    <t>Corrupt Duck Major</t>
-  </si>
-  <si>
-    <t>"Who's going to question a major?"</t>
-  </si>
-  <si>
     <t>Respected Duck Sergeant</t>
   </si>
   <si>
@@ -601,9 +574,6 @@
     <t>Trust me. You want him on your side.</t>
   </si>
   <si>
-    <t>"Where I come from, carving is a contact sport."</t>
-  </si>
-  <si>
     <t>"Did I ever tell you about the time we disabled fourteen flaming barrel mortars?"</t>
   </si>
   <si>
@@ -616,24 +586,12 @@
     <t>"Why would anyone want a clock in their coffin?"</t>
   </si>
   <si>
-    <t>"This must be some sort of pre-historic key chain!!"</t>
-  </si>
-  <si>
     <t>"Please tell me those colors were never popular."</t>
   </si>
   <si>
-    <t>"These spikes don't look very aerodynamic."</t>
-  </si>
-  <si>
     <t>"What's this? A carpet?"</t>
   </si>
   <si>
-    <t>"Who's gonna mess with a guy in this?"</t>
-  </si>
-  <si>
-    <t>"Do you think this is what drove the fish to rebel?"</t>
-  </si>
-  <si>
     <t>"I'm so glad we trashed these things and used paper instead."</t>
   </si>
   <si>
@@ -647,45 +605,22 @@
   </si>
   <si>
     <t>"I'll tell people that she's my sister and she needs gas money."</t>
-  </si>
-  <si>
-    <t>"To be clear, we don't sell fleas. They come free."</t>
   </si>
   <si>
     <t>"I don't think that glass will fit."
 "Challenge accepted!"</t>
   </si>
   <si>
-    <t>"Anyone home?"
-"Yes?"
-"Can I have it?"</t>
-  </si>
-  <si>
     <t>"Who's got two lungs and a trade skill??
 This guy."</t>
   </si>
   <si>
-    <t>"I don't really know why this one is better than yours. I just know it is."</t>
-  </si>
-  <si>
-    <t>"Just let the metal come to me. 
-What could go wrong?"</t>
-  </si>
-  <si>
-    <t>"What's after post-modern? 
-Caveman. Fashion is cyclical."</t>
-  </si>
-  <si>
     <t>"Isn't 'being green' with a submarine just being blue?"</t>
   </si>
   <si>
     <t>"Nobody's gonna miss thes pallets right?"</t>
   </si>
   <si>
-    <t>"I shall call him Mort. 
-He will protect me and carry my junk."</t>
-  </si>
-  <si>
     <t>Bundle of Two-by-Fours</t>
   </si>
   <si>
@@ -693,17 +628,80 @@
   </si>
   <si>
     <t>"You can never have too many windows in a yurt!"</t>
+  </si>
+  <si>
+    <t>"I'll just tell people I'm in a band!"</t>
+  </si>
+  <si>
+    <t>"Who's gonna mess with this polyester?"</t>
+  </si>
+  <si>
+    <t>"Hm, these spikes don't look very aerodynamic."</t>
+  </si>
+  <si>
+    <t>Sack of Brass Door Knobs</t>
+  </si>
+  <si>
+    <t>"Woah. Someone was in a hurry."</t>
+  </si>
+  <si>
+    <t>"Do you think these are what drove the fish to rebel?"</t>
+  </si>
+  <si>
+    <t>"I get it. Don't leave any fingerprints. Smart."</t>
+  </si>
+  <si>
+    <t>"Anyone home?"
+"Yes"
+"Can I have it?"</t>
+  </si>
+  <si>
+    <t>Dilapidated Shack</t>
+  </si>
+  <si>
+    <t>"I don't really know why this one is better than yours. I just know that it is."</t>
+  </si>
+  <si>
+    <t>"I'll just let the metal come to me. What could go wrong?"</t>
+  </si>
+  <si>
+    <t>"What's after post-modern? Caveman. (Fashion is cyclical.)"</t>
+  </si>
+  <si>
+    <t>"To be clear, we do not sell fleas. They come free."</t>
+  </si>
+  <si>
+    <t>"Who would spend their Friday night with stick figure instructions and an allen wrench?"</t>
+  </si>
+  <si>
+    <t>"I shall call him Hillsborough."</t>
+  </si>
+  <si>
+    <t>"None may know the hour of my arrival."</t>
+  </si>
+  <si>
+    <t>"Mutiny is an art form best expressed privately."</t>
+  </si>
+  <si>
+    <t>Sketchy Pirate</t>
+  </si>
+  <si>
+    <t>"Where I come from, we duel to the death. Only you have to carve your weapon first. And neatness counts."</t>
+  </si>
+  <si>
+    <t>"Now with more disease! 
+Pro tip: if you use it on cats, throw them all at once. Otherwise they catch on."</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -3043,16 +3041,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GF58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E52" sqref="E52"/>
+      <selection pane="bottomLeft" activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5" style="74" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.69921875" style="74" bestFit="1" customWidth="1"/>
@@ -3073,7 +3071,7 @@
     <col min="189" max="16384" width="6.59765625" style="75"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:188" s="116" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="1" spans="1:188" s="116" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="108" t="s">
         <v>0</v>
       </c>
@@ -3084,7 +3082,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="110" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E1" s="111" t="s">
         <v>3</v>
@@ -3099,34 +3097,34 @@
         <v>6</v>
       </c>
       <c r="I1" s="113" t="s">
+        <v>122</v>
+      </c>
+      <c r="J1" s="111" t="s">
+        <v>158</v>
+      </c>
+      <c r="K1" s="114" t="s">
+        <v>159</v>
+      </c>
+      <c r="L1" s="114" t="s">
+        <v>160</v>
+      </c>
+      <c r="M1" s="114" t="s">
+        <v>161</v>
+      </c>
+      <c r="N1" s="112" t="s">
         <v>124</v>
       </c>
-      <c r="J1" s="111" t="s">
+      <c r="O1" s="112" t="s">
+        <v>162</v>
+      </c>
+      <c r="P1" s="112" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q1" s="112" t="s">
         <v>164</v>
       </c>
-      <c r="K1" s="114" t="s">
+      <c r="R1" s="112" t="s">
         <v>165</v>
-      </c>
-      <c r="L1" s="114" t="s">
-        <v>166</v>
-      </c>
-      <c r="M1" s="114" t="s">
-        <v>167</v>
-      </c>
-      <c r="N1" s="112" t="s">
-        <v>126</v>
-      </c>
-      <c r="O1" s="112" t="s">
-        <v>168</v>
-      </c>
-      <c r="P1" s="112" t="s">
-        <v>169</v>
-      </c>
-      <c r="Q1" s="112" t="s">
-        <v>170</v>
-      </c>
-      <c r="R1" s="112" t="s">
-        <v>171</v>
       </c>
       <c r="S1" s="115"/>
       <c r="T1" s="115"/>
@@ -3299,7 +3297,7 @@
       <c r="GE1" s="115"/>
       <c r="GF1" s="115"/>
     </row>
-    <row r="2" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="2" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="117" t="s">
         <v>8</v>
       </c>
@@ -3310,7 +3308,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="120" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E2" s="121"/>
       <c r="F2" s="122"/>
@@ -3333,7 +3331,7 @@
       <c r="Q2" s="123"/>
       <c r="R2" s="126"/>
     </row>
-    <row r="3" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="3" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="64" t="s">
         <v>8</v>
       </c>
@@ -3344,7 +3342,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="127" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E3" s="67"/>
       <c r="F3" s="72">
@@ -3369,7 +3367,7 @@
       <c r="Q3" s="72"/>
       <c r="R3" s="73"/>
     </row>
-    <row r="4" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="64" t="s">
         <v>8</v>
       </c>
@@ -3380,7 +3378,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="127" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="E4" s="67"/>
       <c r="F4" s="72">
@@ -3407,18 +3405,18 @@
       <c r="Q4" s="72"/>
       <c r="R4" s="73"/>
     </row>
-    <row r="5" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="5" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="65" t="s">
-        <v>15</v>
+        <v>206</v>
       </c>
       <c r="C5" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="127" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E5" s="70">
         <v>3</v>
@@ -3443,18 +3441,18 @@
       <c r="Q5" s="72"/>
       <c r="R5" s="73"/>
     </row>
-    <row r="6" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="65" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="127" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E6" s="67"/>
       <c r="F6" s="68"/>
@@ -3467,13 +3465,13 @@
         <v>1</v>
       </c>
       <c r="K6" s="71" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="72">
+        <v>1</v>
+      </c>
+      <c r="M6" s="71" t="s">
         <v>17</v>
-      </c>
-      <c r="L6" s="72">
-        <v>1</v>
-      </c>
-      <c r="M6" s="71" t="s">
-        <v>18</v>
       </c>
       <c r="N6" s="72"/>
       <c r="O6" s="72"/>
@@ -3481,18 +3479,18 @@
       <c r="Q6" s="72"/>
       <c r="R6" s="72"/>
     </row>
-    <row r="7" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="7" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="65" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="127" t="s">
-        <v>138</v>
+        <v>203</v>
       </c>
       <c r="E7" s="67"/>
       <c r="F7" s="72">
@@ -3507,7 +3505,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="71" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L7" s="72">
         <v>1</v>
@@ -3521,18 +3519,18 @@
       <c r="Q7" s="72"/>
       <c r="R7" s="72"/>
     </row>
-    <row r="8" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="8" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="65" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="127" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="E8" s="70">
         <v>2</v>
@@ -3559,18 +3557,18 @@
       <c r="Q8" s="72"/>
       <c r="R8" s="73"/>
     </row>
-    <row r="9" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="9" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="65" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="127" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E9" s="70">
         <v>5</v>
@@ -3583,7 +3581,7 @@
         <v>1</v>
       </c>
       <c r="K9" s="71" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L9" s="68"/>
       <c r="M9" s="68"/>
@@ -3593,18 +3591,18 @@
       <c r="Q9" s="72"/>
       <c r="R9" s="73"/>
     </row>
-    <row r="10" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="10" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="65" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="127" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E10" s="70">
         <v>3</v>
@@ -3619,7 +3617,7 @@
         <v>1</v>
       </c>
       <c r="K10" s="71" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L10" s="68"/>
       <c r="M10" s="68"/>
@@ -3629,18 +3627,18 @@
       <c r="Q10" s="72"/>
       <c r="R10" s="73"/>
     </row>
-    <row r="11" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="11" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="65" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="127" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="E11" s="70">
         <v>2</v>
@@ -3661,7 +3659,7 @@
         <v>1</v>
       </c>
       <c r="M11" s="71" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N11" s="72"/>
       <c r="O11" s="72"/>
@@ -3669,18 +3667,18 @@
       <c r="Q11" s="72"/>
       <c r="R11" s="72"/>
     </row>
-    <row r="12" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="12" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="65" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="127" t="s">
-        <v>131</v>
+        <v>207</v>
       </c>
       <c r="E12" s="67"/>
       <c r="F12" s="72">
@@ -3701,18 +3699,18 @@
       <c r="Q12" s="72"/>
       <c r="R12" s="73"/>
     </row>
-    <row r="13" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="13" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="65" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="127" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E13" s="70">
         <v>2</v>
@@ -3727,13 +3725,13 @@
         <v>1</v>
       </c>
       <c r="K13" s="71" t="s">
+        <v>16</v>
+      </c>
+      <c r="L13" s="72">
+        <v>1</v>
+      </c>
+      <c r="M13" s="71" t="s">
         <v>17</v>
-      </c>
-      <c r="L13" s="72">
-        <v>1</v>
-      </c>
-      <c r="M13" s="71" t="s">
-        <v>18</v>
       </c>
       <c r="N13" s="72"/>
       <c r="O13" s="72"/>
@@ -3741,18 +3739,18 @@
       <c r="Q13" s="72"/>
       <c r="R13" s="72"/>
     </row>
-    <row r="14" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="14" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="65" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="127" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="E14" s="67"/>
       <c r="F14" s="72">
@@ -3779,18 +3777,18 @@
       <c r="Q14" s="72"/>
       <c r="R14" s="73"/>
     </row>
-    <row r="15" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="15" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="65" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="127" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E15" s="67"/>
       <c r="F15" s="72">
@@ -3807,7 +3805,7 @@
         <v>1</v>
       </c>
       <c r="K15" s="71" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L15" s="68"/>
       <c r="M15" s="68"/>
@@ -3817,18 +3815,18 @@
       <c r="Q15" s="72"/>
       <c r="R15" s="73"/>
     </row>
-    <row r="16" spans="1:188" ht="17.100000000000001" customHeight="1">
+    <row r="16" spans="1:188" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="65" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="127" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E16" s="67"/>
       <c r="F16" s="68"/>
@@ -3851,18 +3849,18 @@
       <c r="Q16" s="72"/>
       <c r="R16" s="73"/>
     </row>
-    <row r="17" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="17" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="65" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="127" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E17" s="70">
         <v>3</v>
@@ -3883,18 +3881,18 @@
       <c r="Q17" s="72"/>
       <c r="R17" s="73"/>
     </row>
-    <row r="18" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="18" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="65" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="127" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="E18" s="67"/>
       <c r="F18" s="68"/>
@@ -3919,18 +3917,18 @@
       <c r="Q18" s="72"/>
       <c r="R18" s="73"/>
     </row>
-    <row r="19" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="19" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="65" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="127" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E19" s="67"/>
       <c r="F19" s="72">
@@ -3945,7 +3943,7 @@
         <v>1</v>
       </c>
       <c r="K19" s="71" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L19" s="72"/>
       <c r="M19" s="71"/>
@@ -3955,18 +3953,18 @@
       <c r="Q19" s="72"/>
       <c r="R19" s="72"/>
     </row>
-    <row r="20" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="20" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="65" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="127" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E20" s="70">
         <v>4</v>
@@ -3987,18 +3985,18 @@
       <c r="Q20" s="72"/>
       <c r="R20" s="73"/>
     </row>
-    <row r="21" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="21" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="65" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D21" s="127" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="E21" s="70">
         <v>2</v>
@@ -4015,7 +4013,7 @@
         <v>1</v>
       </c>
       <c r="K21" s="71" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L21" s="68"/>
       <c r="M21" s="68"/>
@@ -4025,18 +4023,18 @@
       <c r="Q21" s="72"/>
       <c r="R21" s="73"/>
     </row>
-    <row r="22" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="22" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="65" t="s">
-        <v>37</v>
+        <v>211</v>
       </c>
       <c r="C22" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="127" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E22" s="70">
         <v>3</v>
@@ -4059,18 +4057,18 @@
       <c r="Q22" s="72"/>
       <c r="R22" s="73"/>
     </row>
-    <row r="23" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="23" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B23" s="65" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C23" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D23" s="127" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="E23" s="70">
         <v>3</v>
@@ -4087,7 +4085,7 @@
         <v>1</v>
       </c>
       <c r="K23" s="71" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L23" s="68"/>
       <c r="M23" s="68"/>
@@ -4097,18 +4095,18 @@
       <c r="Q23" s="72"/>
       <c r="R23" s="73"/>
     </row>
-    <row r="24" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="24" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B24" s="65" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C24" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D24" s="127" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="E24" s="70">
         <v>2</v>
@@ -4131,18 +4129,18 @@
       <c r="Q24" s="72"/>
       <c r="R24" s="73"/>
     </row>
-    <row r="25" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="25" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B25" s="65" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C25" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D25" s="127" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E25" s="70">
         <v>2</v>
@@ -4167,18 +4165,18 @@
       <c r="Q25" s="72"/>
       <c r="R25" s="73"/>
     </row>
-    <row r="26" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="26" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B26" s="65" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C26" s="66" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D26" s="127" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E26" s="67"/>
       <c r="F26" s="68"/>
@@ -4199,18 +4197,18 @@
       <c r="Q26" s="72"/>
       <c r="R26" s="73"/>
     </row>
-    <row r="27" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="27" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B27" s="65" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C27" s="66" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D27" s="127" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E27" s="70">
         <v>5</v>
@@ -4233,18 +4231,18 @@
       <c r="Q27" s="72"/>
       <c r="R27" s="73"/>
     </row>
-    <row r="28" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="28" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B28" s="139" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="C28" s="66" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D28" s="127" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E28" s="70">
         <v>2</v>
@@ -4259,7 +4257,7 @@
         <v>1</v>
       </c>
       <c r="K28" s="71" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L28" s="68"/>
       <c r="M28" s="68"/>
@@ -4269,18 +4267,18 @@
       <c r="Q28" s="72"/>
       <c r="R28" s="73"/>
     </row>
-    <row r="29" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="29" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B29" s="65" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C29" s="66" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D29" s="127" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E29" s="67"/>
       <c r="F29" s="72">
@@ -4305,18 +4303,18 @@
       <c r="Q29" s="72"/>
       <c r="R29" s="73"/>
     </row>
-    <row r="30" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="30" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B30" s="65" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C30" s="66" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D30" s="127" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E30" s="70">
         <v>1</v>
@@ -4343,18 +4341,18 @@
       <c r="Q30" s="72"/>
       <c r="R30" s="73"/>
     </row>
-    <row r="31" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="31" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B31" s="65" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C31" s="66" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D31" s="127" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E31" s="70">
         <v>3</v>
@@ -4379,18 +4377,18 @@
       <c r="Q31" s="72"/>
       <c r="R31" s="73"/>
     </row>
-    <row r="32" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="32" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B32" s="65" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C32" s="66" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D32" s="127" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E32" s="67"/>
       <c r="F32" s="72">
@@ -4415,18 +4413,18 @@
       <c r="Q32" s="72"/>
       <c r="R32" s="73"/>
     </row>
-    <row r="33" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="33" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B33" s="65" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C33" s="66" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D33" s="127" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="E33" s="70">
         <v>3</v>
@@ -4449,18 +4447,18 @@
       <c r="Q33" s="72"/>
       <c r="R33" s="73"/>
     </row>
-    <row r="34" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="34" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B34" s="65" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C34" s="66" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D34" s="127" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E34" s="70">
         <v>2</v>
@@ -4483,18 +4481,18 @@
       <c r="Q34" s="72"/>
       <c r="R34" s="73"/>
     </row>
-    <row r="35" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="35" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B35" s="65" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C35" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D35" s="127" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E35" s="67"/>
       <c r="F35" s="68"/>
@@ -4509,13 +4507,13 @@
         <v>1</v>
       </c>
       <c r="K35" s="71" t="s">
+        <v>16</v>
+      </c>
+      <c r="L35" s="72">
+        <v>1</v>
+      </c>
+      <c r="M35" s="71" t="s">
         <v>17</v>
-      </c>
-      <c r="L35" s="72">
-        <v>1</v>
-      </c>
-      <c r="M35" s="71" t="s">
-        <v>18</v>
       </c>
       <c r="N35" s="72"/>
       <c r="O35" s="72"/>
@@ -4523,18 +4521,18 @@
       <c r="Q35" s="72"/>
       <c r="R35" s="72"/>
     </row>
-    <row r="36" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="36" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="65" t="s">
         <v>50</v>
-      </c>
-      <c r="B36" s="65" t="s">
-        <v>52</v>
       </c>
       <c r="C36" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D36" s="127" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E36" s="67"/>
       <c r="F36" s="72">
@@ -4549,13 +4547,13 @@
         <v>1</v>
       </c>
       <c r="K36" s="71" t="s">
+        <v>16</v>
+      </c>
+      <c r="L36" s="72">
+        <v>1</v>
+      </c>
+      <c r="M36" s="71" t="s">
         <v>17</v>
-      </c>
-      <c r="L36" s="72">
-        <v>1</v>
-      </c>
-      <c r="M36" s="71" t="s">
-        <v>18</v>
       </c>
       <c r="N36" s="72"/>
       <c r="O36" s="72"/>
@@ -4563,18 +4561,18 @@
       <c r="Q36" s="72"/>
       <c r="R36" s="72"/>
     </row>
-    <row r="37" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="37" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B37" s="65" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C37" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D37" s="127" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E37" s="67"/>
       <c r="F37" s="72">
@@ -4591,13 +4589,13 @@
         <v>2</v>
       </c>
       <c r="K37" s="71" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L37" s="72">
         <v>2</v>
       </c>
       <c r="M37" s="71" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N37" s="72"/>
       <c r="O37" s="72"/>
@@ -4605,18 +4603,18 @@
       <c r="Q37" s="72"/>
       <c r="R37" s="72"/>
     </row>
-    <row r="38" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="38" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B38" s="65" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C38" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D38" s="127" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E38" s="70">
         <v>2</v>
@@ -4633,13 +4631,13 @@
         <v>3</v>
       </c>
       <c r="K38" s="71" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L38" s="72">
         <v>1</v>
       </c>
       <c r="M38" s="71" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N38" s="72"/>
       <c r="O38" s="72"/>
@@ -4647,18 +4645,18 @@
       <c r="Q38" s="72"/>
       <c r="R38" s="72"/>
     </row>
-    <row r="39" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="39" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B39" s="65" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C39" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D39" s="127" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E39" s="67"/>
       <c r="F39" s="68"/>
@@ -4677,7 +4675,7 @@
         <v>2</v>
       </c>
       <c r="M39" s="71" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N39" s="72"/>
       <c r="O39" s="72"/>
@@ -4685,18 +4683,18 @@
       <c r="Q39" s="72"/>
       <c r="R39" s="72"/>
     </row>
-    <row r="40" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="40" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B40" s="65" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C40" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D40" s="127" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E40" s="70">
         <v>2</v>
@@ -4714,13 +4712,13 @@
       <c r="L40" s="129"/>
       <c r="M40" s="68"/>
       <c r="N40" s="129" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="O40" s="72">
         <v>1</v>
       </c>
       <c r="P40" s="73" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="Q40" s="72">
         <v>1</v>
@@ -4729,18 +4727,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="41" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B41" s="65" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C41" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D41" s="127" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E41" s="70">
         <v>2</v>
@@ -4758,13 +4756,13 @@
       <c r="L41" s="129"/>
       <c r="M41" s="68"/>
       <c r="N41" s="129" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="O41" s="72">
         <v>1</v>
       </c>
       <c r="P41" s="73" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="Q41" s="72">
         <v>1</v>
@@ -4773,18 +4771,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="42" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B42" s="65" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C42" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D42" s="127" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E42" s="67"/>
       <c r="F42" s="68"/>
@@ -4801,7 +4799,7 @@
         <v>3</v>
       </c>
       <c r="K42" s="71" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L42" s="68"/>
       <c r="M42" s="68"/>
@@ -4811,18 +4809,18 @@
       <c r="Q42" s="72"/>
       <c r="R42" s="73"/>
     </row>
-    <row r="43" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="43" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B43" s="65" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C43" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D43" s="127" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E43" s="67"/>
       <c r="F43" s="72">
@@ -4839,7 +4837,7 @@
         <v>3</v>
       </c>
       <c r="K43" s="76" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L43" s="68"/>
       <c r="M43" s="68"/>
@@ -4849,18 +4847,18 @@
       <c r="Q43" s="72"/>
       <c r="R43" s="73"/>
     </row>
-    <row r="44" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="44" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B44" s="77" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C44" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D44" s="127" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="E44" s="70">
         <v>4</v>
@@ -4885,18 +4883,18 @@
       <c r="Q44" s="72"/>
       <c r="R44" s="73"/>
     </row>
-    <row r="45" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="45" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B45" s="77" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C45" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D45" s="127" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E45" s="70">
         <v>4</v>
@@ -4919,18 +4917,18 @@
       <c r="Q45" s="72"/>
       <c r="R45" s="73"/>
     </row>
-    <row r="46" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="46" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B46" s="77" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C46" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D46" s="127" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E46" s="70">
         <v>2</v>
@@ -4951,7 +4949,7 @@
         <v>1</v>
       </c>
       <c r="M46" s="71" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N46" s="72"/>
       <c r="O46" s="72"/>
@@ -4959,18 +4957,18 @@
       <c r="Q46" s="72"/>
       <c r="R46" s="72"/>
     </row>
-    <row r="47" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="47" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B47" s="77" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C47" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D47" s="127" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E47" s="70">
         <v>12</v>
@@ -4985,7 +4983,7 @@
       </c>
       <c r="J47" s="67"/>
       <c r="K47" s="71" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L47" s="68"/>
       <c r="M47" s="68"/>
@@ -4995,18 +4993,18 @@
       <c r="Q47" s="72"/>
       <c r="R47" s="73"/>
     </row>
-    <row r="48" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="48" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B48" s="77" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C48" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D48" s="127" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E48" s="67"/>
       <c r="F48" s="72">
@@ -5021,7 +5019,7 @@
       </c>
       <c r="J48" s="67"/>
       <c r="K48" s="71" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L48" s="68"/>
       <c r="M48" s="68"/>
@@ -5031,18 +5029,18 @@
       <c r="Q48" s="72"/>
       <c r="R48" s="73"/>
     </row>
-    <row r="49" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="49" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B49" s="65" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C49" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D49" s="127" t="s">
-        <v>159</v>
+        <v>222</v>
       </c>
       <c r="E49" s="70">
         <v>12</v>
@@ -5057,7 +5055,7 @@
       </c>
       <c r="J49" s="67"/>
       <c r="K49" s="71" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L49" s="68"/>
       <c r="M49" s="68"/>
@@ -5067,18 +5065,18 @@
       <c r="Q49" s="72"/>
       <c r="R49" s="73"/>
     </row>
-    <row r="50" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="50" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B50" s="77" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C50" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D50" s="127" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="E50" s="67"/>
       <c r="F50" s="68"/>
@@ -5093,7 +5091,7 @@
       </c>
       <c r="J50" s="67"/>
       <c r="K50" s="71" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L50" s="68"/>
       <c r="M50" s="68"/>
@@ -5103,18 +5101,18 @@
       <c r="Q50" s="72"/>
       <c r="R50" s="73"/>
     </row>
-    <row r="51" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="51" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B51" s="65" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C51" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D51" s="127" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E51" s="67"/>
       <c r="F51" s="72">
@@ -5129,7 +5127,7 @@
       </c>
       <c r="J51" s="67"/>
       <c r="K51" s="71" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L51" s="68"/>
       <c r="M51" s="68"/>
@@ -5139,18 +5137,18 @@
       <c r="Q51" s="72"/>
       <c r="R51" s="73"/>
     </row>
-    <row r="52" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="52" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B52" s="65" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="C52" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D52" s="127" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="E52" s="70">
         <v>12</v>
@@ -5165,7 +5163,7 @@
       </c>
       <c r="J52" s="67"/>
       <c r="K52" s="71" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L52" s="68"/>
       <c r="M52" s="68"/>
@@ -5175,18 +5173,18 @@
       <c r="Q52" s="72"/>
       <c r="R52" s="73"/>
     </row>
-    <row r="53" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="53" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B53" s="65" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C53" s="66" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D53" s="127" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E53" s="70">
         <v>2</v>
@@ -5201,13 +5199,13 @@
         <v>2</v>
       </c>
       <c r="K53" s="71" t="s">
+        <v>16</v>
+      </c>
+      <c r="L53" s="72">
+        <v>1</v>
+      </c>
+      <c r="M53" s="71" t="s">
         <v>17</v>
-      </c>
-      <c r="L53" s="72">
-        <v>1</v>
-      </c>
-      <c r="M53" s="71" t="s">
-        <v>18</v>
       </c>
       <c r="N53" s="72"/>
       <c r="O53" s="72"/>
@@ -5215,18 +5213,18 @@
       <c r="Q53" s="72"/>
       <c r="R53" s="72"/>
     </row>
-    <row r="54" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="54" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B54" s="65" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C54" s="66" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D54" s="127" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="E54" s="67"/>
       <c r="F54" s="68"/>
@@ -5245,7 +5243,7 @@
         <v>1</v>
       </c>
       <c r="M54" s="71" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N54" s="72"/>
       <c r="O54" s="72"/>
@@ -5253,18 +5251,18 @@
       <c r="Q54" s="72"/>
       <c r="R54" s="72"/>
     </row>
-    <row r="55" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="55" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B55" s="65" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C55" s="66" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D55" s="127" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E55" s="67"/>
       <c r="F55" s="72">
@@ -5283,7 +5281,7 @@
         <v>1</v>
       </c>
       <c r="M55" s="71" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N55" s="72"/>
       <c r="O55" s="72"/>
@@ -5291,18 +5289,18 @@
       <c r="Q55" s="72"/>
       <c r="R55" s="72"/>
     </row>
-    <row r="56" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="56" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B56" s="65" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C56" s="66" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D56" s="127" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="E56" s="70">
         <v>2</v>
@@ -5322,33 +5320,33 @@
       <c r="L56" s="72"/>
       <c r="M56" s="68"/>
       <c r="N56" s="72" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="O56" s="72">
         <v>1</v>
       </c>
       <c r="P56" s="73" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="Q56" s="72">
         <v>1</v>
       </c>
       <c r="R56" s="73" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18" ht="17.100000000000001" customHeight="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B57" s="65" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C57" s="66" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D57" s="127" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E57" s="67"/>
       <c r="F57" s="68"/>
@@ -5371,18 +5369,18 @@
       <c r="Q57" s="72"/>
       <c r="R57" s="73"/>
     </row>
-    <row r="58" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="58" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B58" s="65" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C58" s="66" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D58" s="127" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E58" s="67"/>
       <c r="F58" s="72">
@@ -5403,7 +5401,7 @@
         <v>1</v>
       </c>
       <c r="M58" s="71" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N58" s="72"/>
       <c r="O58" s="72"/>
@@ -5439,14 +5437,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IK16"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.796875" style="89" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.09765625" style="89" bestFit="1" customWidth="1"/>
@@ -5465,7 +5463,7 @@
     <col min="18" max="16384" width="8.796875" style="89"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:245" s="107" customFormat="1" ht="15">
+    <row r="1" spans="1:245" s="107" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="107" t="s">
         <v>0</v>
       </c>
@@ -5476,60 +5474,60 @@
         <v>2</v>
       </c>
       <c r="D1" s="135" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E1" s="107" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="F1" s="107" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="G1" s="107" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="H1" s="107" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="I1" s="111" t="s">
+        <v>158</v>
+      </c>
+      <c r="J1" s="114" t="s">
+        <v>159</v>
+      </c>
+      <c r="K1" s="114" t="s">
+        <v>160</v>
+      </c>
+      <c r="L1" s="114" t="s">
+        <v>161</v>
+      </c>
+      <c r="M1" s="112" t="s">
+        <v>124</v>
+      </c>
+      <c r="N1" s="112" t="s">
+        <v>162</v>
+      </c>
+      <c r="O1" s="112" t="s">
+        <v>163</v>
+      </c>
+      <c r="P1" s="112" t="s">
         <v>164</v>
       </c>
-      <c r="J1" s="114" t="s">
+      <c r="Q1" s="112" t="s">
         <v>165</v>
       </c>
-      <c r="K1" s="114" t="s">
-        <v>166</v>
-      </c>
-      <c r="L1" s="114" t="s">
-        <v>167</v>
-      </c>
-      <c r="M1" s="112" t="s">
-        <v>126</v>
-      </c>
-      <c r="N1" s="112" t="s">
-        <v>168</v>
-      </c>
-      <c r="O1" s="112" t="s">
-        <v>169</v>
-      </c>
-      <c r="P1" s="112" t="s">
-        <v>170</v>
-      </c>
-      <c r="Q1" s="112" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="2" spans="1:245" ht="17.100000000000001" customHeight="1">
+    </row>
+    <row r="2" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="78" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B2" s="79" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C2" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="134" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E2" s="81"/>
       <c r="F2" s="82"/>
@@ -5540,13 +5538,13 @@
       <c r="K2" s="86"/>
       <c r="L2" s="82"/>
       <c r="M2" s="86" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="N2" s="86">
         <v>2</v>
       </c>
       <c r="O2" s="87" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="P2" s="86">
         <v>1</v>
@@ -5783,18 +5781,18 @@
       <c r="IJ2" s="88"/>
       <c r="IK2" s="88"/>
     </row>
-    <row r="3" spans="1:245" ht="17.100000000000001" customHeight="1">
+    <row r="3" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="78" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B3" s="79" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="C3" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="134" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="E3" s="84">
         <v>1</v>
@@ -5813,13 +5811,13 @@
       <c r="K3" s="86"/>
       <c r="L3" s="82"/>
       <c r="M3" s="86" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="N3" s="86">
         <v>1</v>
       </c>
       <c r="O3" s="87" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="P3" s="86">
         <v>1</v>
@@ -6056,18 +6054,18 @@
       <c r="IJ3" s="88"/>
       <c r="IK3" s="88"/>
     </row>
-    <row r="4" spans="1:245" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="78" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B4" s="79" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="C4" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="134" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E4" s="84">
         <v>1</v>
@@ -6086,13 +6084,13 @@
       <c r="K4" s="86"/>
       <c r="L4" s="82"/>
       <c r="M4" s="86" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="N4" s="86">
         <v>1</v>
       </c>
       <c r="O4" s="87" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="P4" s="86">
         <v>1</v>
@@ -6329,18 +6327,18 @@
       <c r="IJ4" s="88"/>
       <c r="IK4" s="88"/>
     </row>
-    <row r="5" spans="1:245" ht="17.100000000000001" customHeight="1">
+    <row r="5" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="78" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B5" s="79" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C5" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="134" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E5" s="84">
         <v>1</v>
@@ -6355,13 +6353,13 @@
       <c r="K5" s="86"/>
       <c r="L5" s="82"/>
       <c r="M5" s="86" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="N5" s="86">
         <v>1</v>
       </c>
       <c r="O5" s="87" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="P5" s="86">
         <v>2</v>
@@ -6598,18 +6596,18 @@
       <c r="IJ5" s="88"/>
       <c r="IK5" s="88"/>
     </row>
-    <row r="6" spans="1:245" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="78" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B6" s="79" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C6" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="134" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E6" s="81"/>
       <c r="F6" s="82"/>
@@ -6619,7 +6617,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="85" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K6" s="82"/>
       <c r="L6" s="82"/>
@@ -6857,18 +6855,18 @@
       <c r="IJ6" s="88"/>
       <c r="IK6" s="88"/>
     </row>
-    <row r="7" spans="1:245" ht="17.100000000000001" customHeight="1">
+    <row r="7" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="78" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B7" s="79" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C7" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="134" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E7" s="84">
         <v>2</v>
@@ -6883,7 +6881,7 @@
       <c r="K7" s="86"/>
       <c r="L7" s="82"/>
       <c r="M7" s="86" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="N7" s="86">
         <v>1</v>
@@ -7126,18 +7124,18 @@
       <c r="IJ7" s="88"/>
       <c r="IK7" s="88"/>
     </row>
-    <row r="8" spans="1:245" ht="17.100000000000001" customHeight="1">
+    <row r="8" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="78" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B8" s="79" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C8" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="134" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E8" s="81"/>
       <c r="F8" s="82"/>
@@ -7385,18 +7383,18 @@
       <c r="IJ8" s="88"/>
       <c r="IK8" s="88"/>
     </row>
-    <row r="9" spans="1:245" ht="17.100000000000001" customHeight="1">
+    <row r="9" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="78" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B9" s="79" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="C9" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="138" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="E9" s="84">
         <v>3</v>
@@ -7411,7 +7409,7 @@
       <c r="K9" s="86"/>
       <c r="L9" s="82"/>
       <c r="M9" s="86" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="N9" s="86">
         <v>1</v>
@@ -7423,7 +7421,7 @@
         <v>1</v>
       </c>
       <c r="Q9" s="87" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="R9" s="88"/>
       <c r="S9" s="88"/>
@@ -7654,18 +7652,18 @@
       <c r="IJ9" s="88"/>
       <c r="IK9" s="88"/>
     </row>
-    <row r="10" spans="1:245" ht="17.100000000000001" customHeight="1">
+    <row r="10" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="78" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B10" s="79" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C10" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="134" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E10" s="84">
         <v>1</v>
@@ -7679,7 +7677,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="90" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="K10" s="86"/>
       <c r="L10" s="85"/>
@@ -7917,18 +7915,18 @@
       <c r="IJ10" s="88"/>
       <c r="IK10" s="88"/>
     </row>
-    <row r="11" spans="1:245" ht="17.100000000000001" customHeight="1">
+    <row r="11" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="78" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B11" s="79" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C11" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="134" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E11" s="84">
         <v>2</v>
@@ -7948,7 +7946,7 @@
         <v>1</v>
       </c>
       <c r="L11" s="85" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M11" s="86"/>
       <c r="N11" s="86"/>
@@ -8184,18 +8182,18 @@
       <c r="IJ11" s="88"/>
       <c r="IK11" s="88"/>
     </row>
-    <row r="12" spans="1:245" ht="17.100000000000001" customHeight="1">
+    <row r="12" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="78" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B12" s="79" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C12" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="134" t="s">
-        <v>186</v>
+        <v>218</v>
       </c>
       <c r="E12" s="84">
         <v>2</v>
@@ -8210,19 +8208,19 @@
       <c r="K12" s="86"/>
       <c r="L12" s="82"/>
       <c r="M12" s="86" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="N12" s="86">
         <v>1</v>
       </c>
       <c r="O12" s="87" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="P12" s="86">
         <v>1</v>
       </c>
       <c r="Q12" s="87" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="R12" s="88"/>
       <c r="S12" s="88"/>
@@ -8453,18 +8451,18 @@
       <c r="IJ12" s="88"/>
       <c r="IK12" s="88"/>
     </row>
-    <row r="13" spans="1:245" ht="17.100000000000001" customHeight="1">
+    <row r="13" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="78" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B13" s="92" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C13" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="134" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="E13" s="93"/>
       <c r="F13" s="82"/>
@@ -8472,7 +8470,7 @@
       <c r="H13" s="83"/>
       <c r="I13" s="84"/>
       <c r="J13" s="85" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="K13" s="87"/>
       <c r="L13" s="94"/>
@@ -8710,18 +8708,18 @@
       <c r="IJ13" s="88"/>
       <c r="IK13" s="88"/>
     </row>
-    <row r="14" spans="1:245" ht="17.100000000000001" customHeight="1">
+    <row r="14" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="78" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B14" s="92" t="s">
-        <v>188</v>
+        <v>220</v>
       </c>
       <c r="C14" s="80" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D14" s="134" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="E14" s="84">
         <v>1</v>
@@ -8736,13 +8734,13 @@
       <c r="K14" s="86"/>
       <c r="L14" s="85"/>
       <c r="M14" s="86" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="N14" s="86">
         <v>1</v>
       </c>
       <c r="O14" s="86" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="P14" s="86">
         <v>1</v>
@@ -8979,18 +8977,18 @@
       <c r="IJ14" s="88"/>
       <c r="IK14" s="88"/>
     </row>
-    <row r="15" spans="1:245" ht="17.100000000000001" customHeight="1">
+    <row r="15" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="78" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B15" s="92" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C15" s="80" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D15" s="134" t="s">
-        <v>194</v>
+        <v>221</v>
       </c>
       <c r="E15" s="84">
         <v>2</v>
@@ -9005,7 +9003,7 @@
       <c r="K15" s="86"/>
       <c r="L15" s="94"/>
       <c r="M15" s="86" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="N15" s="86">
         <v>1</v>
@@ -9017,7 +9015,7 @@
         <v>1</v>
       </c>
       <c r="Q15" s="87" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="R15" s="88"/>
       <c r="S15" s="88"/>
@@ -9248,18 +9246,18 @@
       <c r="IJ15" s="88"/>
       <c r="IK15" s="88"/>
     </row>
-    <row r="16" spans="1:245" s="106" customFormat="1" ht="15.75" customHeight="1">
+    <row r="16" spans="1:245" s="106" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="97" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B16" s="98" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C16" s="99" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D16" s="136" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="E16" s="100">
         <v>1</v>
@@ -9273,7 +9271,7 @@
         <v>1</v>
       </c>
       <c r="J16" s="101" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K16" s="104">
         <v>1</v>
@@ -9539,12 +9537,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.59765625" style="23" customWidth="1"/>
     <col min="2" max="2" width="9" style="23" customWidth="1"/>
@@ -9553,7 +9551,7 @@
     <col min="5" max="256" width="6.59765625" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="1" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>1</v>
       </c>
@@ -9561,295 +9559,295 @@
         <v>0</v>
       </c>
       <c r="C1" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="6"/>
-    </row>
-    <row r="2" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A2" s="26" t="s">
+      <c r="C2" s="27" t="s">
         <v>94</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>96</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="3" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>95</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>97</v>
       </c>
       <c r="D3" s="29"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D4" s="29"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="5" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D5" s="29"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D6" s="29"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="7" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="8" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="9" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C9" s="29"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="10" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C10" s="29"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="11" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C11" s="29"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="12" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="13" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C13" s="29"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="14" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C14" s="29"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="15" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C15" s="29"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="16" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C16" s="29"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="17" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C17" s="29"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="18" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C18" s="29"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="19" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C19" s="29"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="20" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D20" s="32"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="21" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="33" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D21" s="34"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="22" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B22" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>104</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>106</v>
       </c>
       <c r="D22" s="29"/>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="23" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D23" s="29"/>
       <c r="E23" s="6"/>
     </row>
-    <row r="24" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="24" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D24" s="29"/>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="25" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D25" s="29"/>
       <c r="E25" s="6"/>
@@ -9864,14 +9862,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.3984375" style="35" customWidth="1"/>
     <col min="2" max="2" width="6.8984375" style="35" customWidth="1"/>
@@ -9889,26 +9887,26 @@
     <col min="15" max="256" width="6.59765625" style="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="1" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="144" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B1" s="141"/>
       <c r="C1" s="140" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D1" s="145"/>
       <c r="E1" s="141"/>
       <c r="F1" s="140" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G1" s="141"/>
       <c r="H1" s="140" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I1" s="141"/>
       <c r="J1" s="140" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K1" s="141"/>
       <c r="L1" s="29"/>
@@ -9919,7 +9917,7 @@
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
     </row>
-    <row r="2" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="2" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -9927,37 +9925,37 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>118</v>
       </c>
       <c r="N2" s="37"/>
       <c r="O2" s="6"/>
@@ -9965,7 +9963,7 @@
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
     </row>
-    <row r="3" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="3" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="str">
         <f>Primitives!A3</f>
         <v>initiative</v>
@@ -10003,7 +10001,7 @@
       <c r="Q3" s="6"/>
       <c r="R3" s="6"/>
     </row>
-    <row r="4" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="str">
         <f>Primitives!A4</f>
         <v>capacity</v>
@@ -10041,7 +10039,7 @@
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
     </row>
-    <row r="5" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="5" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="17"/>
       <c r="C5" s="16"/>
@@ -10073,7 +10071,7 @@
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
     </row>
-    <row r="6" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="44" t="str">
         <f>Primitives!A20</f>
         <v>take one</v>
@@ -10111,7 +10109,7 @@
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="7" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="str">
         <f>Primitives!A24</f>
         <v>string</v>
@@ -10165,7 +10163,7 @@
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
     </row>
-    <row r="8" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="8" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="str">
         <f>Primitives!A25</f>
         <v>wood</v>
@@ -10220,7 +10218,7 @@
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
     </row>
-    <row r="9" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="9" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="str">
         <f>Primitives!A23</f>
         <v>metal</v>
@@ -10275,7 +10273,7 @@
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
     </row>
-    <row r="10" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="10" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
@@ -10329,7 +10327,7 @@
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
     </row>
-    <row r="11" spans="1:18" ht="15.75" customHeight="1">
+    <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="str">
         <f>Primitives!A21</f>
         <v>duct tape</v>
@@ -10384,7 +10382,7 @@
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
     </row>
-    <row r="12" spans="1:18" ht="16.5" customHeight="1">
+    <row r="12" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="48"/>
       <c r="C12" s="49"/>
@@ -10404,22 +10402,22 @@
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
     </row>
-    <row r="13" spans="1:18" ht="15.75" customHeight="1">
+    <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="E13" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="F13" s="140" t="s">
         <v>119</v>
-      </c>
-      <c r="E13" s="53" t="s">
-        <v>120</v>
-      </c>
-      <c r="F13" s="140" t="s">
-        <v>121</v>
       </c>
       <c r="G13" s="141"/>
       <c r="H13" s="142" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I13" s="143"/>
       <c r="J13" s="42"/>
@@ -10432,12 +10430,12 @@
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="14" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="54">
@@ -10474,12 +10472,12 @@
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
     </row>
-    <row r="15" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="15" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="54">
@@ -10516,12 +10514,12 @@
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
     </row>
-    <row r="16" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="16" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="54">
@@ -10558,12 +10556,12 @@
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
     </row>
-    <row r="17" spans="1:18" ht="15.75" customHeight="1">
+    <row r="17" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="45" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C17" s="32"/>
       <c r="D17" s="59">
@@ -10600,7 +10598,7 @@
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
     </row>
-    <row r="18" spans="1:18" ht="15.75" customHeight="1">
+    <row r="18" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -10615,7 +10613,7 @@
       <c r="L18" s="6"/>
       <c r="M18" s="11"/>
       <c r="N18" s="63" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="O18" s="6"/>
       <c r="P18" s="4" t="s">
@@ -10628,7 +10626,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="19" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -10659,7 +10657,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="20" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -10687,7 +10685,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="17.100000000000001" customHeight="1">
+    <row r="21" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>

</xml_diff>

<commit_message>
Punching up the snarks
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -457,9 +457,6 @@
     <t>Reformed Tree Gnome</t>
   </si>
   <si>
-    <t>"Good for catching people and tree gnomes!"</t>
-  </si>
-  <si>
     <t>"Do you expect me to etch this? No, I expect you to DIE!"</t>
   </si>
   <si>
@@ -691,6 +688,9 @@
   <si>
     <t>"Now with more disease! 
 Pro tip: if you use it on cats, throw them all at once. Otherwise they catch on."</t>
+  </si>
+  <si>
+    <t>"Good for catching a man, or multiple tree gnomes!"</t>
   </si>
 </sst>
 </file>
@@ -3045,9 +3045,9 @@
   <dimension ref="A1:GF58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D50" sqref="D50"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3100,31 +3100,31 @@
         <v>122</v>
       </c>
       <c r="J1" s="111" t="s">
+        <v>157</v>
+      </c>
+      <c r="K1" s="114" t="s">
         <v>158</v>
       </c>
-      <c r="K1" s="114" t="s">
+      <c r="L1" s="114" t="s">
         <v>159</v>
       </c>
-      <c r="L1" s="114" t="s">
+      <c r="M1" s="114" t="s">
         <v>160</v>
-      </c>
-      <c r="M1" s="114" t="s">
-        <v>161</v>
       </c>
       <c r="N1" s="112" t="s">
         <v>124</v>
       </c>
       <c r="O1" s="112" t="s">
+        <v>161</v>
+      </c>
+      <c r="P1" s="112" t="s">
         <v>162</v>
       </c>
-      <c r="P1" s="112" t="s">
+      <c r="Q1" s="112" t="s">
         <v>163</v>
       </c>
-      <c r="Q1" s="112" t="s">
+      <c r="R1" s="112" t="s">
         <v>164</v>
-      </c>
-      <c r="R1" s="112" t="s">
-        <v>165</v>
       </c>
       <c r="S1" s="115"/>
       <c r="T1" s="115"/>
@@ -3378,7 +3378,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="127" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E4" s="67"/>
       <c r="F4" s="72">
@@ -3410,13 +3410,13 @@
         <v>8</v>
       </c>
       <c r="B5" s="65" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C5" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="127" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E5" s="70">
         <v>3</v>
@@ -3490,7 +3490,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="127" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E7" s="67"/>
       <c r="F7" s="72">
@@ -3530,7 +3530,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="127" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E8" s="70">
         <v>2</v>
@@ -3568,7 +3568,7 @@
         <v>10</v>
       </c>
       <c r="D9" s="127" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E9" s="70">
         <v>5</v>
@@ -3602,7 +3602,7 @@
         <v>10</v>
       </c>
       <c r="D10" s="127" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E10" s="70">
         <v>3</v>
@@ -3638,7 +3638,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="127" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E11" s="70">
         <v>2</v>
@@ -3678,7 +3678,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="127" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E12" s="67"/>
       <c r="F12" s="72">
@@ -3750,7 +3750,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="127" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E14" s="67"/>
       <c r="F14" s="72">
@@ -3892,7 +3892,7 @@
         <v>10</v>
       </c>
       <c r="D18" s="127" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E18" s="67"/>
       <c r="F18" s="68"/>
@@ -3996,7 +3996,7 @@
         <v>10</v>
       </c>
       <c r="D21" s="127" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E21" s="70">
         <v>2</v>
@@ -4028,13 +4028,13 @@
         <v>8</v>
       </c>
       <c r="B22" s="65" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C22" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="127" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E22" s="70">
         <v>3</v>
@@ -4068,7 +4068,7 @@
         <v>10</v>
       </c>
       <c r="D23" s="127" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E23" s="70">
         <v>3</v>
@@ -4106,7 +4106,7 @@
         <v>10</v>
       </c>
       <c r="D24" s="127" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E24" s="70">
         <v>2</v>
@@ -4140,7 +4140,7 @@
         <v>10</v>
       </c>
       <c r="D25" s="127" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E25" s="70">
         <v>2</v>
@@ -4236,7 +4236,7 @@
         <v>8</v>
       </c>
       <c r="B28" s="139" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C28" s="66" t="s">
         <v>40</v>
@@ -4424,7 +4424,7 @@
         <v>40</v>
       </c>
       <c r="D33" s="127" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E33" s="70">
         <v>3</v>
@@ -4572,7 +4572,7 @@
         <v>10</v>
       </c>
       <c r="D37" s="127" t="s">
-        <v>146</v>
+        <v>222</v>
       </c>
       <c r="E37" s="67"/>
       <c r="F37" s="72">
@@ -4614,7 +4614,7 @@
         <v>10</v>
       </c>
       <c r="D38" s="127" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E38" s="70">
         <v>2</v>
@@ -4656,7 +4656,7 @@
         <v>10</v>
       </c>
       <c r="D39" s="127" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E39" s="67"/>
       <c r="F39" s="68"/>
@@ -4694,7 +4694,7 @@
         <v>10</v>
       </c>
       <c r="D40" s="127" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E40" s="70">
         <v>2</v>
@@ -4738,7 +4738,7 @@
         <v>10</v>
       </c>
       <c r="D41" s="127" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E41" s="70">
         <v>2</v>
@@ -4782,7 +4782,7 @@
         <v>10</v>
       </c>
       <c r="D42" s="127" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E42" s="67"/>
       <c r="F42" s="68"/>
@@ -4820,7 +4820,7 @@
         <v>10</v>
       </c>
       <c r="D43" s="127" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E43" s="67"/>
       <c r="F43" s="72">
@@ -4858,7 +4858,7 @@
         <v>10</v>
       </c>
       <c r="D44" s="127" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E44" s="70">
         <v>4</v>
@@ -4894,7 +4894,7 @@
         <v>10</v>
       </c>
       <c r="D45" s="127" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E45" s="70">
         <v>4</v>
@@ -4928,7 +4928,7 @@
         <v>10</v>
       </c>
       <c r="D46" s="127" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E46" s="70">
         <v>2</v>
@@ -4968,7 +4968,7 @@
         <v>10</v>
       </c>
       <c r="D47" s="127" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E47" s="70">
         <v>12</v>
@@ -5004,7 +5004,7 @@
         <v>10</v>
       </c>
       <c r="D48" s="127" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E48" s="67"/>
       <c r="F48" s="72">
@@ -5040,7 +5040,7 @@
         <v>10</v>
       </c>
       <c r="D49" s="127" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E49" s="70">
         <v>12</v>
@@ -5076,7 +5076,7 @@
         <v>10</v>
       </c>
       <c r="D50" s="127" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E50" s="67"/>
       <c r="F50" s="68"/>
@@ -5112,7 +5112,7 @@
         <v>10</v>
       </c>
       <c r="D51" s="127" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E51" s="67"/>
       <c r="F51" s="72">
@@ -5142,13 +5142,13 @@
         <v>48</v>
       </c>
       <c r="B52" s="65" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C52" s="66" t="s">
         <v>10</v>
       </c>
       <c r="D52" s="127" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E52" s="70">
         <v>12</v>
@@ -5184,7 +5184,7 @@
         <v>40</v>
       </c>
       <c r="D53" s="127" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E53" s="70">
         <v>2</v>
@@ -5224,7 +5224,7 @@
         <v>40</v>
       </c>
       <c r="D54" s="127" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E54" s="67"/>
       <c r="F54" s="68"/>
@@ -5262,7 +5262,7 @@
         <v>40</v>
       </c>
       <c r="D55" s="127" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E55" s="67"/>
       <c r="F55" s="72">
@@ -5300,7 +5300,7 @@
         <v>40</v>
       </c>
       <c r="D56" s="127" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E56" s="70">
         <v>2</v>
@@ -5346,7 +5346,7 @@
         <v>40</v>
       </c>
       <c r="D57" s="127" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E57" s="67"/>
       <c r="F57" s="68"/>
@@ -5380,7 +5380,7 @@
         <v>40</v>
       </c>
       <c r="D58" s="127" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E58" s="67"/>
       <c r="F58" s="72">
@@ -5477,43 +5477,43 @@
         <v>125</v>
       </c>
       <c r="E1" s="107" t="s">
+        <v>165</v>
+      </c>
+      <c r="F1" s="107" t="s">
         <v>166</v>
       </c>
-      <c r="F1" s="107" t="s">
+      <c r="G1" s="107" t="s">
         <v>167</v>
       </c>
-      <c r="G1" s="107" t="s">
+      <c r="H1" s="107" t="s">
         <v>168</v>
       </c>
-      <c r="H1" s="107" t="s">
-        <v>169</v>
-      </c>
       <c r="I1" s="111" t="s">
+        <v>157</v>
+      </c>
+      <c r="J1" s="114" t="s">
         <v>158</v>
       </c>
-      <c r="J1" s="114" t="s">
+      <c r="K1" s="114" t="s">
         <v>159</v>
       </c>
-      <c r="K1" s="114" t="s">
+      <c r="L1" s="114" t="s">
         <v>160</v>
-      </c>
-      <c r="L1" s="114" t="s">
-        <v>161</v>
       </c>
       <c r="M1" s="112" t="s">
         <v>124</v>
       </c>
       <c r="N1" s="112" t="s">
+        <v>161</v>
+      </c>
+      <c r="O1" s="112" t="s">
         <v>162</v>
       </c>
-      <c r="O1" s="112" t="s">
+      <c r="P1" s="112" t="s">
         <v>163</v>
       </c>
-      <c r="P1" s="112" t="s">
+      <c r="Q1" s="112" t="s">
         <v>164</v>
-      </c>
-      <c r="Q1" s="112" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:245" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -5521,13 +5521,13 @@
         <v>76</v>
       </c>
       <c r="B2" s="79" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C2" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="134" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E2" s="81"/>
       <c r="F2" s="82"/>
@@ -5786,13 +5786,13 @@
         <v>76</v>
       </c>
       <c r="B3" s="79" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C3" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="134" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E3" s="84">
         <v>1</v>
@@ -6059,13 +6059,13 @@
         <v>76</v>
       </c>
       <c r="B4" s="79" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C4" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="134" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E4" s="84">
         <v>1</v>
@@ -6338,7 +6338,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="134" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E5" s="84">
         <v>1</v>
@@ -6607,7 +6607,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="134" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E6" s="81"/>
       <c r="F6" s="82"/>
@@ -6860,13 +6860,13 @@
         <v>76</v>
       </c>
       <c r="B7" s="79" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C7" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="134" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E7" s="84">
         <v>2</v>
@@ -7135,7 +7135,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="134" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E8" s="81"/>
       <c r="F8" s="82"/>
@@ -7388,13 +7388,13 @@
         <v>76</v>
       </c>
       <c r="B9" s="79" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C9" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="138" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E9" s="84">
         <v>3</v>
@@ -7663,7 +7663,7 @@
         <v>10</v>
       </c>
       <c r="D10" s="134" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E10" s="84">
         <v>1</v>
@@ -7677,7 +7677,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K10" s="86"/>
       <c r="L10" s="85"/>
@@ -7926,7 +7926,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="134" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E11" s="84">
         <v>2</v>
@@ -8193,7 +8193,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="134" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E12" s="84">
         <v>2</v>
@@ -8462,7 +8462,7 @@
         <v>10</v>
       </c>
       <c r="D13" s="134" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E13" s="93"/>
       <c r="F13" s="82"/>
@@ -8470,7 +8470,7 @@
       <c r="H13" s="83"/>
       <c r="I13" s="84"/>
       <c r="J13" s="85" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K13" s="87"/>
       <c r="L13" s="94"/>
@@ -8713,13 +8713,13 @@
         <v>76</v>
       </c>
       <c r="B14" s="92" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C14" s="80" t="s">
         <v>40</v>
       </c>
       <c r="D14" s="134" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E14" s="84">
         <v>1</v>
@@ -8988,7 +8988,7 @@
         <v>40</v>
       </c>
       <c r="D15" s="134" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E15" s="84">
         <v>2</v>
@@ -9257,7 +9257,7 @@
         <v>40</v>
       </c>
       <c r="D16" s="136" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E16" s="100">
         <v>1</v>

</xml_diff>